<commit_message>
fixed the name of the last operation, it's INSERT: edges-specific.ru
</commit_message>
<xml_diff>
--- a/leaks-load.xlsx
+++ b/leaks-load.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>file</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>INSERT: edges-specific.ru</t>
   </si>
 </sst>
 </file>
@@ -1104,7 +1107,7 @@
   <dimension ref="B1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1601,7 +1604,7 @@
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
after the insert of the jurisdiction links
</commit_message>
<xml_diff>
--- a/leaks-load.xlsx
+++ b/leaks-load.xlsx
@@ -13,8 +13,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+MUST be run after countries-link next time</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>file</t>
   </si>
@@ -122,18 +158,47 @@
   </si>
   <si>
     <t>INSERT: edges-specific.ru</t>
+  </si>
+  <si>
+    <t>INSERT: jurisdictions-link.ru</t>
+  </si>
+  <si>
+    <t>on import</t>
+  </si>
+  <si>
+    <t>leaks:countries-link</t>
+  </si>
+  <si>
+    <t>leaks:jurisdictions-link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -145,45 +210,48 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="204"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="204"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="42">
     <border>
@@ -733,72 +801,75 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1103,18 +1174,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="M17" sqref="M17:Q17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.21875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.21875" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" style="1" customWidth="1"/>
@@ -1122,119 +1193,122 @@
     <col min="8" max="8" width="11" style="1" customWidth="1"/>
     <col min="9" max="9" width="10.5546875" style="1" customWidth="1"/>
     <col min="10" max="10" width="11.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" style="1"/>
-    <col min="12" max="12" width="9.109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" style="1" customWidth="1"/>
     <col min="14" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B2" s="8"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="20" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="19" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="20" t="s">
+      <c r="G2" s="7"/>
+      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="52" t="s">
+      <c r="I2" s="8"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="52" t="s">
+      <c r="L2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="52" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13" t="s">
+      <c r="K3" s="16"/>
+      <c r="L3" s="16" t="s">
         <v>24</v>
+      </c>
+      <c r="M3" s="53" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="19">
         <v>0</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="20">
         <v>80</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="21">
         <v>870</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="22">
         <v>1272</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="19">
         <f>F4-D4</f>
         <v>870</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="23">
         <f>J4-H4</f>
         <v>322</v>
       </c>
-      <c r="J4" s="22">
+      <c r="J4" s="20">
         <f>G4-E4</f>
         <v>1192</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="24">
         <v>0.7</v>
       </c>
-      <c r="L4" s="30">
+      <c r="L4" s="25">
         <f>H4/K4</f>
         <v>1242.8571428571429</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="18" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="26">
@@ -1251,31 +1325,31 @@
       <c r="G5" s="29">
         <v>2817150</v>
       </c>
-      <c r="H5" s="21">
+      <c r="H5" s="19">
         <f>F5-D5</f>
         <v>2470270</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="23">
         <f>J5-H5</f>
         <v>345608</v>
       </c>
-      <c r="J5" s="22">
+      <c r="J5" s="20">
         <f>G5-E5</f>
         <v>2815878</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5" s="24">
         <v>54.6</v>
       </c>
-      <c r="L5" s="30">
+      <c r="L5" s="25">
         <f t="shared" ref="L5:L7" si="0">H5/K5</f>
         <v>45243.040293040292</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="18" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="26">
@@ -1292,31 +1366,31 @@
       <c r="G6" s="29">
         <v>3038593</v>
       </c>
-      <c r="H6" s="21">
+      <c r="H6" s="19">
         <f>F6-D6</f>
         <v>197801</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="23">
         <f>J6-H6</f>
         <v>23642</v>
       </c>
-      <c r="J6" s="22">
+      <c r="J6" s="20">
         <f>G6-E6</f>
         <v>221443</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="24">
         <v>4.5999999999999996</v>
       </c>
-      <c r="L6" s="30">
+      <c r="L6" s="25">
         <f t="shared" si="0"/>
         <v>43000.217391304352</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="18" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="26">
@@ -1327,37 +1401,37 @@
         <f>G6</f>
         <v>3038593</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="19">
         <v>7902266</v>
       </c>
       <c r="G7" s="29">
         <v>8591092</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="19">
         <f>F7-D7</f>
         <v>5233325</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="23">
         <f>J7-H7</f>
         <v>319174</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7" s="20">
         <f>G7-E7</f>
         <v>5552499</v>
       </c>
-      <c r="K7" s="14">
+      <c r="K7" s="24">
         <v>126.3</v>
       </c>
-      <c r="L7" s="30">
+      <c r="L7" s="25">
         <f t="shared" si="0"/>
         <v>41435.669041963578</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="18" t="s">
         <v>26</v>
       </c>
       <c r="D8" s="26">
@@ -1374,31 +1448,31 @@
       <c r="G8" s="29">
         <v>13670282</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="19">
         <f>F8-D8</f>
         <v>5079184</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I8" s="23">
         <f>J8-H8</f>
         <v>6</v>
       </c>
-      <c r="J8" s="22">
+      <c r="J8" s="20">
         <f>G8-E8</f>
         <v>5079190</v>
       </c>
-      <c r="K8" s="14">
+      <c r="K8" s="24">
         <v>123.6</v>
       </c>
-      <c r="L8" s="30">
+      <c r="L8" s="25">
         <f t="shared" ref="L8" si="1">H8/K8</f>
         <v>41093.7216828479</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="26">
@@ -1415,68 +1489,68 @@
       <c r="G9" s="29">
         <v>15626835</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="19">
         <f t="shared" ref="H9:H15" si="4">F9-D9</f>
         <v>1956549</v>
       </c>
-      <c r="I9" s="25">
-        <f t="shared" ref="I9:I16" si="5">J9-H9</f>
+      <c r="I9" s="23">
+        <f t="shared" ref="I9:I15" si="5">J9-H9</f>
         <v>4</v>
       </c>
-      <c r="J9" s="22">
+      <c r="J9" s="20">
         <f t="shared" ref="J9:J15" si="6">G9-E9</f>
         <v>1956553</v>
       </c>
-      <c r="K9" s="14">
+      <c r="K9" s="24">
         <v>49.5</v>
       </c>
-      <c r="L9" s="30">
+      <c r="L9" s="25">
         <f t="shared" ref="L9:L15" si="7">H9/K9</f>
         <v>39526.242424242424</v>
       </c>
-      <c r="M9" s="31">
+      <c r="M9" s="30">
         <v>1956549</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="18" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="27"/>
       <c r="F10" s="28"/>
       <c r="G10" s="29"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="30"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="25"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="18" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="26"/>
       <c r="E11" s="27"/>
       <c r="F11" s="28"/>
       <c r="G11" s="29"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="30"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="25"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="18" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="26">
@@ -1493,32 +1567,32 @@
       <c r="G12" s="29">
         <v>15628207</v>
       </c>
-      <c r="H12" s="21">
+      <c r="H12" s="19">
         <f t="shared" si="4"/>
         <v>1033</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="23">
         <f t="shared" si="5"/>
         <v>339</v>
       </c>
-      <c r="J12" s="22">
+      <c r="J12" s="20">
         <f t="shared" si="6"/>
         <v>1372</v>
       </c>
-      <c r="K12" s="14">
+      <c r="K12" s="24">
         <v>0.2</v>
       </c>
-      <c r="L12" s="30">
+      <c r="L12" s="25">
         <f t="shared" si="7"/>
         <v>5165</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>27</v>
+      <c r="C13" s="55" t="s">
+        <v>38</v>
       </c>
       <c r="D13" s="26">
         <f>F9</f>
@@ -1534,26 +1608,26 @@
       <c r="G13" s="29">
         <v>16590188</v>
       </c>
-      <c r="H13" s="21">
+      <c r="H13" s="19">
         <f>F13-D13</f>
         <v>641733</v>
       </c>
-      <c r="I13" s="25">
+      <c r="I13" s="23">
         <f>J13-H13</f>
         <v>321620</v>
       </c>
-      <c r="J13" s="22">
+      <c r="J13" s="20">
         <f>G13-E13</f>
         <v>963353</v>
       </c>
-      <c r="K13" s="14">
+      <c r="K13" s="24">
         <v>136.4</v>
       </c>
-      <c r="L13" s="30">
+      <c r="L13" s="25">
         <f>H13/K13</f>
         <v>4704.7873900293253</v>
       </c>
-      <c r="M13" s="31">
+      <c r="M13" s="30">
         <f>640700</f>
         <v>640700</v>
       </c>
@@ -1562,10 +1636,10 @@
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="18" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="26">
@@ -1582,31 +1656,31 @@
       <c r="G14" s="29">
         <v>17235242</v>
       </c>
-      <c r="H14" s="21">
+      <c r="H14" s="19">
         <f t="shared" si="4"/>
         <v>1203294</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I14" s="23">
         <f t="shared" si="5"/>
         <v>403741</v>
       </c>
-      <c r="J14" s="22">
+      <c r="J14" s="20">
         <f t="shared" si="6"/>
         <v>1607035</v>
       </c>
-      <c r="K14" s="14">
+      <c r="K14" s="24">
         <v>18.899999999999999</v>
       </c>
-      <c r="L14" s="30">
+      <c r="L14" s="25">
         <f t="shared" si="7"/>
         <v>63666.349206349209</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="31" t="s">
         <v>33</v>
       </c>
       <c r="D15" s="26">
@@ -1623,26 +1697,26 @@
       <c r="G15" s="29">
         <v>19758781</v>
       </c>
-      <c r="H15" s="21">
+      <c r="H15" s="19">
         <f t="shared" si="4"/>
         <v>1005149</v>
       </c>
-      <c r="I15" s="25">
+      <c r="I15" s="23">
         <f t="shared" si="5"/>
         <v>1518390</v>
       </c>
-      <c r="J15" s="22">
+      <c r="J15" s="20">
         <f t="shared" si="6"/>
         <v>2523539</v>
       </c>
-      <c r="K15" s="14">
+      <c r="K15" s="24">
         <v>67.099999999999994</v>
       </c>
-      <c r="L15" s="30">
+      <c r="L15" s="25">
         <f t="shared" si="7"/>
         <v>14979.865871833086</v>
       </c>
-      <c r="M15" s="31">
+      <c r="M15" s="30">
         <f>1004149</f>
         <v>1004149</v>
       </c>
@@ -1650,54 +1724,96 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="32"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="41"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="31">
-        <f>1004149</f>
-        <v>1004149</v>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B16" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="26">
+        <f>F15</f>
+        <v>17147475</v>
+      </c>
+      <c r="E16" s="27">
+        <f>G15</f>
+        <v>19758781</v>
+      </c>
+      <c r="F16" s="28">
+        <v>17466625</v>
+      </c>
+      <c r="G16" s="28">
+        <v>20077933</v>
+      </c>
+      <c r="H16" s="19">
+        <f>F16-D16</f>
+        <v>319150</v>
+      </c>
+      <c r="I16" s="23">
+        <f>J16-H16</f>
+        <v>2</v>
+      </c>
+      <c r="J16" s="20">
+        <f>G16-E16</f>
+        <v>319152</v>
+      </c>
+      <c r="K16" s="24">
+        <v>136.4</v>
+      </c>
+      <c r="L16" s="25">
+        <f>H16/K16</f>
+        <v>2339.8093841642226</v>
+      </c>
+      <c r="M16" s="30">
+        <f>319150</f>
+        <v>319150</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:12" s="43" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="44" t="s">
+    <row r="17" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="32"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="30"/>
+    </row>
+    <row r="18" spans="2:13" s="51" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="46">
-        <f>SUM(H4:H16)</f>
-        <v>17789208</v>
-      </c>
-      <c r="I17" s="50">
-        <f>SUM(I4:I16)</f>
-        <v>2932846</v>
-      </c>
-      <c r="J17" s="47">
-        <f>SUM(J4:J16)</f>
-        <v>20722054</v>
-      </c>
-      <c r="K17" s="44">
-        <f>SUM(K4:K16)</f>
-        <v>581.9</v>
-      </c>
-      <c r="L17" s="51">
-        <f>H17/K17</f>
-        <v>30570.902216875755</v>
+      <c r="C18" s="44"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="45">
+        <f>SUM(H4:H17)</f>
+        <v>18108358</v>
+      </c>
+      <c r="I18" s="49">
+        <f>SUM(I4:I17)</f>
+        <v>2932848</v>
+      </c>
+      <c r="J18" s="46">
+        <f>SUM(J4:J17)</f>
+        <v>21041206</v>
+      </c>
+      <c r="K18" s="43">
+        <f>SUM(K4:K17)</f>
+        <v>718.3</v>
+      </c>
+      <c r="L18" s="50">
+        <f>H18/K18</f>
+        <v>25210.020882639568</v>
       </c>
     </row>
   </sheetData>
@@ -1712,8 +1828,10 @@
     <hyperlink ref="C4" r:id="rId3" display="http://data.ontotext.com/resource/leaks/ontology"/>
     <hyperlink ref="C6:C8" r:id="rId4" display="http://data.ontotext.com/resource/leaks/raw-data"/>
     <hyperlink ref="C11:C14" r:id="rId5" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
+    <hyperlink ref="C16" r:id="rId6" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967294" r:id="rId7"/>
+  <legacyDrawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed the formulas for the totals
</commit_message>
<xml_diff>
--- a/leaks-load.xlsx
+++ b/leaks-load.xlsx
@@ -1178,7 +1178,7 @@
   <dimension ref="B1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17:Q17"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1595,12 +1595,12 @@
         <v>38</v>
       </c>
       <c r="D13" s="26">
-        <f>F9</f>
-        <v>14937999</v>
+        <f>F12</f>
+        <v>14939032</v>
       </c>
       <c r="E13" s="27">
-        <f>G9</f>
-        <v>15626835</v>
+        <f>G12</f>
+        <v>15628207</v>
       </c>
       <c r="F13" s="28">
         <v>15579732</v>
@@ -1610,22 +1610,22 @@
       </c>
       <c r="H13" s="19">
         <f>F13-D13</f>
-        <v>641733</v>
+        <v>640700</v>
       </c>
       <c r="I13" s="23">
         <f>J13-H13</f>
-        <v>321620</v>
+        <v>321281</v>
       </c>
       <c r="J13" s="20">
         <f>G13-E13</f>
-        <v>963353</v>
+        <v>961981</v>
       </c>
       <c r="K13" s="24">
         <v>136.4</v>
       </c>
       <c r="L13" s="25">
         <f>H13/K13</f>
-        <v>4704.7873900293253</v>
+        <v>4697.2140762463341</v>
       </c>
       <c r="M13" s="30">
         <f>640700</f>
@@ -1643,12 +1643,12 @@
         <v>17</v>
       </c>
       <c r="D14" s="26">
-        <f>F12</f>
-        <v>14939032</v>
+        <f t="shared" ref="D14:D16" si="8">F13</f>
+        <v>15579732</v>
       </c>
       <c r="E14" s="27">
-        <f>G12</f>
-        <v>15628207</v>
+        <f t="shared" ref="E14:E16" si="9">G13</f>
+        <v>16590188</v>
       </c>
       <c r="F14" s="28">
         <v>16142326</v>
@@ -1658,22 +1658,22 @@
       </c>
       <c r="H14" s="19">
         <f t="shared" si="4"/>
-        <v>1203294</v>
+        <v>562594</v>
       </c>
       <c r="I14" s="23">
         <f t="shared" si="5"/>
-        <v>403741</v>
+        <v>82460</v>
       </c>
       <c r="J14" s="20">
         <f t="shared" si="6"/>
-        <v>1607035</v>
+        <v>645054</v>
       </c>
       <c r="K14" s="24">
         <v>18.899999999999999</v>
       </c>
       <c r="L14" s="25">
         <f t="shared" si="7"/>
-        <v>63666.349206349209</v>
+        <v>29766.878306878309</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
@@ -1684,11 +1684,11 @@
         <v>33</v>
       </c>
       <c r="D15" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>16142326</v>
       </c>
       <c r="E15" s="27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>17235242</v>
       </c>
       <c r="F15" s="28">
@@ -1732,11 +1732,11 @@
         <v>39</v>
       </c>
       <c r="D16" s="26">
-        <f>F15</f>
+        <f t="shared" si="8"/>
         <v>17147475</v>
       </c>
       <c r="E16" s="27">
-        <f>G15</f>
+        <f t="shared" si="9"/>
         <v>19758781</v>
       </c>
       <c r="F16" s="28">
@@ -1796,16 +1796,16 @@
       <c r="F18" s="47"/>
       <c r="G18" s="48"/>
       <c r="H18" s="45">
-        <f>SUM(H4:H17)</f>
-        <v>18108358</v>
+        <f>SUM(H4:H17)+D4</f>
+        <v>17466625</v>
       </c>
       <c r="I18" s="49">
-        <f>SUM(I4:I17)</f>
-        <v>2932848</v>
+        <f>SUM(I4:I17)+(E4-D4)</f>
+        <v>2611308</v>
       </c>
       <c r="J18" s="46">
-        <f>SUM(J4:J17)</f>
-        <v>21041206</v>
+        <f>SUM(J4:J17)+E4</f>
+        <v>20077933</v>
       </c>
       <c r="K18" s="43">
         <f>SUM(K4:K17)</f>
@@ -1813,7 +1813,7 @@
       </c>
       <c r="L18" s="50">
         <f>H18/K18</f>
-        <v>25210.020882639568</v>
+        <v>24316.615620214397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
after the load of skos.rdf
</commit_message>
<xml_diff>
--- a/leaks-load.xlsx
+++ b/leaks-load.xlsx
@@ -45,12 +45,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="B17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+MUST be loaded before leak-ontology.ttl</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>file</t>
   </si>
@@ -170,6 +196,12 @@
   </si>
   <si>
     <t>leaks:jurisdictions-link</t>
+  </si>
+  <si>
+    <t>skos.rdf</t>
+  </si>
+  <si>
+    <t>leaks:skos-schema</t>
   </si>
 </sst>
 </file>
@@ -1175,10 +1207,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N18"/>
+  <dimension ref="B1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1476,11 +1508,11 @@
         <v>27</v>
       </c>
       <c r="D9" s="26">
-        <f t="shared" ref="D9:D15" si="2">F8</f>
+        <f t="shared" ref="D9" si="2">F8</f>
         <v>12981450</v>
       </c>
       <c r="E9" s="27">
-        <f t="shared" ref="E9:E15" si="3">G8</f>
+        <f t="shared" ref="E9" si="3">G8</f>
         <v>13670282</v>
       </c>
       <c r="F9" s="28">
@@ -1772,48 +1804,90 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="32"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="42"/>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B17" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="26">
+        <f t="shared" ref="D17" si="10">F16</f>
+        <v>17466625</v>
+      </c>
+      <c r="E17" s="27">
+        <f t="shared" ref="E17" si="11">G16</f>
+        <v>20077933</v>
+      </c>
+      <c r="F17" s="28">
+        <v>17466877</v>
+      </c>
+      <c r="G17" s="28">
+        <v>20078985</v>
+      </c>
+      <c r="H17" s="19">
+        <f>F17-D17</f>
+        <v>252</v>
+      </c>
+      <c r="I17" s="23">
+        <f>J17-H17</f>
+        <v>800</v>
+      </c>
+      <c r="J17" s="20">
+        <f>G17-E17</f>
+        <v>1052</v>
+      </c>
+      <c r="K17" s="24">
+        <v>136.4</v>
+      </c>
+      <c r="L17" s="25">
+        <f>H17/K17</f>
+        <v>1.847507331378299</v>
+      </c>
       <c r="M17" s="30"/>
     </row>
-    <row r="18" spans="2:13" s="51" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="43" t="s">
+    <row r="18" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="32"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="41"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="30"/>
+    </row>
+    <row r="19" spans="2:13" s="51" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="45">
-        <f>SUM(H4:H17)+D4</f>
-        <v>17466625</v>
-      </c>
-      <c r="I18" s="49">
-        <f>SUM(I4:I17)+(E4-D4)</f>
-        <v>2611308</v>
-      </c>
-      <c r="J18" s="46">
-        <f>SUM(J4:J17)+E4</f>
-        <v>20077933</v>
-      </c>
-      <c r="K18" s="43">
-        <f>SUM(K4:K17)</f>
-        <v>718.3</v>
-      </c>
-      <c r="L18" s="50">
-        <f>H18/K18</f>
-        <v>24316.615620214397</v>
+      <c r="C19" s="44"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="45">
+        <f>SUM(H4:H18)+D4</f>
+        <v>17466877</v>
+      </c>
+      <c r="I19" s="49">
+        <f>SUM(I4:I18)+(E4-D4)</f>
+        <v>2612108</v>
+      </c>
+      <c r="J19" s="46">
+        <f>SUM(J4:J18)+E4</f>
+        <v>20078985</v>
+      </c>
+      <c r="K19" s="43">
+        <f>SUM(K4:K18)</f>
+        <v>854.69999999999993</v>
+      </c>
+      <c r="L19" s="50">
+        <f>H19/K19</f>
+        <v>20436.266526266529</v>
       </c>
     </row>
   </sheetData>
@@ -1829,9 +1903,10 @@
     <hyperlink ref="C6:C8" r:id="rId4" display="http://data.ontotext.com/resource/leaks/raw-data"/>
     <hyperlink ref="C11:C14" r:id="rId5" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
     <hyperlink ref="C16" r:id="rId6" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
+    <hyperlink ref="C17" r:id="rId7" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967294" r:id="rId7"/>
-  <legacyDrawing r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967294" r:id="rId8"/>
+  <legacyDrawing r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
because we have forgotten to load Addresses.ttl on time, we had to load it last and than to run some INSERTS for linking again For the next load, the table will look better
</commit_message>
<xml_diff>
--- a/leaks-load.xlsx
+++ b/leaks-load.xlsx
@@ -19,6 +19,32 @@
     <author>Author</author>
   </authors>
   <commentList>
+    <comment ref="B9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+addresses were not linked, because they were not loaded properly beforehand</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B16" authorId="0" shapeId="0">
       <text>
         <r>
@@ -71,12 +97,116 @@
         </r>
       </text>
     </comment>
+    <comment ref="B18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+MUST be loaded before INSERT: edges-link.ru</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+run second time only because of the ommission of addresses load initially; should be removed for the next load</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+run second time only because of the ommission of addresses load initially; should be removed for the next load</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B21" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+run second time only because of the ommission of addresses load initially; should be removed for the next load</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>file</t>
   </si>
@@ -202,6 +332,12 @@
   </si>
   <si>
     <t>leaks:skos-schema</t>
+  </si>
+  <si>
+    <t>addresses.ttl</t>
+  </si>
+  <si>
+    <t>leaks:raw-data-addresses</t>
   </si>
 </sst>
 </file>
@@ -1207,10 +1343,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N19"/>
+  <dimension ref="B1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1752,9 +1888,6 @@
         <f>1004149</f>
         <v>1004149</v>
       </c>
-      <c r="N15" s="1" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B16" s="54" t="s">
@@ -1804,7 +1937,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="54" t="s">
         <v>40</v>
       </c>
@@ -1838,56 +1971,233 @@
         <v>1052</v>
       </c>
       <c r="K17" s="24">
-        <v>136.4</v>
+        <v>0.1</v>
       </c>
       <c r="L17" s="25">
         <f>H17/K17</f>
-        <v>1.847507331378299</v>
+        <v>2520</v>
       </c>
       <c r="M17" s="30"/>
     </row>
-    <row r="18" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="32"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="42"/>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B18" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="26">
+        <f t="shared" ref="D18:D20" si="12">F17</f>
+        <v>17466877</v>
+      </c>
+      <c r="E18" s="27">
+        <f t="shared" ref="E18:E20" si="13">G17</f>
+        <v>20078985</v>
+      </c>
+      <c r="F18" s="28">
+        <v>18432297</v>
+      </c>
+      <c r="G18" s="28">
+        <v>21169222</v>
+      </c>
+      <c r="H18" s="19">
+        <f>F18-D18</f>
+        <v>965420</v>
+      </c>
+      <c r="I18" s="23">
+        <f>J18-H18</f>
+        <v>124817</v>
+      </c>
+      <c r="J18" s="20">
+        <f>G18-E18</f>
+        <v>1090237</v>
+      </c>
+      <c r="K18" s="24">
+        <v>31.3</v>
+      </c>
+      <c r="L18" s="25">
+        <f>H18/K18</f>
+        <v>30844.089456869009</v>
+      </c>
       <c r="M18" s="30"/>
     </row>
-    <row r="19" spans="2:13" s="51" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="43" t="s">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B19" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="26">
+        <f t="shared" si="12"/>
+        <v>18432297</v>
+      </c>
+      <c r="E19" s="27">
+        <f t="shared" si="13"/>
+        <v>21169222</v>
+      </c>
+      <c r="F19" s="28">
+        <v>18831233</v>
+      </c>
+      <c r="G19" s="29">
+        <v>21568158</v>
+      </c>
+      <c r="H19" s="19">
+        <f t="shared" ref="H19:H20" si="14">F19-D19</f>
+        <v>398936</v>
+      </c>
+      <c r="I19" s="23">
+        <f t="shared" ref="I19:I20" si="15">J19-H19</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="20">
+        <f t="shared" ref="J19:J20" si="16">G19-E19</f>
+        <v>398936</v>
+      </c>
+      <c r="K19" s="24">
+        <v>28.5</v>
+      </c>
+      <c r="L19" s="25">
+        <f t="shared" ref="L19:L20" si="17">H19/K19</f>
+        <v>13997.754385964912</v>
+      </c>
+      <c r="M19" s="30">
+        <v>398936</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B20" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="26">
+        <f t="shared" si="12"/>
+        <v>18831233</v>
+      </c>
+      <c r="E20" s="27">
+        <f t="shared" si="13"/>
+        <v>21568158</v>
+      </c>
+      <c r="F20" s="28">
+        <v>19031024</v>
+      </c>
+      <c r="G20" s="29">
+        <v>21769051</v>
+      </c>
+      <c r="H20" s="19">
+        <f t="shared" si="14"/>
+        <v>199791</v>
+      </c>
+      <c r="I20" s="23">
+        <f t="shared" si="15"/>
+        <v>1102</v>
+      </c>
+      <c r="J20" s="20">
+        <f t="shared" si="16"/>
+        <v>200893</v>
+      </c>
+      <c r="K20" s="24">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="L20" s="25">
+        <f t="shared" si="17"/>
+        <v>11038.17679558011</v>
+      </c>
+      <c r="M20" s="30">
+        <v>199791</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B21" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="26">
+        <f>F20</f>
+        <v>19031024</v>
+      </c>
+      <c r="E21" s="27">
+        <f>G20</f>
+        <v>21769051</v>
+      </c>
+      <c r="F21" s="28">
+        <v>19154932</v>
+      </c>
+      <c r="G21" s="29">
+        <v>21956551</v>
+      </c>
+      <c r="H21" s="19">
+        <f>F21-D21</f>
+        <v>123908</v>
+      </c>
+      <c r="I21" s="23">
+        <f>J21-H21</f>
+        <v>63592</v>
+      </c>
+      <c r="J21" s="20">
+        <f>G21-E21</f>
+        <v>187500</v>
+      </c>
+      <c r="K21" s="24">
+        <v>153</v>
+      </c>
+      <c r="L21" s="25">
+        <f>H21/K21</f>
+        <v>809.85620915032678</v>
+      </c>
+      <c r="M21" s="30">
+        <v>123908</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="32"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="41"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="30"/>
+    </row>
+    <row r="23" spans="2:14" s="51" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="44"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="45">
-        <f>SUM(H4:H18)+D4</f>
-        <v>17466877</v>
-      </c>
-      <c r="I19" s="49">
-        <f>SUM(I4:I18)+(E4-D4)</f>
-        <v>2612108</v>
-      </c>
-      <c r="J19" s="46">
-        <f>SUM(J4:J18)+E4</f>
-        <v>20078985</v>
-      </c>
-      <c r="K19" s="43">
-        <f>SUM(K4:K18)</f>
-        <v>854.69999999999993</v>
-      </c>
-      <c r="L19" s="50">
-        <f>H19/K19</f>
-        <v>20436.266526266529</v>
+      <c r="C23" s="44"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="45">
+        <f>SUM(H4:H22)+D4</f>
+        <v>19154932</v>
+      </c>
+      <c r="I23" s="49">
+        <f>SUM(I4:I22)+(E4-D4)</f>
+        <v>2801619</v>
+      </c>
+      <c r="J23" s="46">
+        <f>SUM(J4:J22)+E4</f>
+        <v>21956551</v>
+      </c>
+      <c r="K23" s="43">
+        <f>SUM(K4:K22)</f>
+        <v>949.3</v>
+      </c>
+      <c r="L23" s="50">
+        <f>H23/K23</f>
+        <v>20177.954282102604</v>
       </c>
     </row>
   </sheetData>
@@ -1904,9 +2214,11 @@
     <hyperlink ref="C11:C14" r:id="rId5" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
     <hyperlink ref="C16" r:id="rId6" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
     <hyperlink ref="C17" r:id="rId7" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
+    <hyperlink ref="C18" r:id="rId8" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
+    <hyperlink ref="C21" r:id="rId9" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967294" r:id="rId8"/>
-  <legacyDrawing r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967294" r:id="rId10"/>
+  <legacyDrawing r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
after loading aux fixes to the ontology
</commit_message>
<xml_diff>
--- a/leaks-load.xlsx
+++ b/leaks-load.xlsx
@@ -201,12 +201,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="B22" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+patch the ontology to provide superClassOff owl:Class for classes that are not linked to the class hierarchy; for the sake getting correct Class Hierarchy diagram. This will be reverted, when the diagram is fixed, because as is it introduces useless inference</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
   <si>
     <t>file</t>
   </si>
@@ -338,6 +364,9 @@
   </si>
   <si>
     <t>leaks:raw-data-addresses</t>
+  </si>
+  <si>
+    <t>….</t>
   </si>
 </sst>
 </file>
@@ -976,21 +1005,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1038,6 +1052,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1343,10 +1372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N23"/>
+  <dimension ref="B1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1371,431 +1400,431 @@
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="52"/>
+      <c r="F2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="54"/>
+      <c r="H2" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="5"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="52"/>
       <c r="K2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="52" t="s">
+      <c r="M2" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="52" t="s">
+      <c r="N2" s="47" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16" t="s">
+      <c r="K3" s="11"/>
+      <c r="L3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="53" t="s">
+      <c r="M3" s="48" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="14">
         <v>0</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="15">
         <v>80</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="16">
         <v>870</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="17">
         <v>1272</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="14">
         <f>F4-D4</f>
         <v>870</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="18">
         <f>J4-H4</f>
         <v>322</v>
       </c>
-      <c r="J4" s="20">
+      <c r="J4" s="15">
         <f>G4-E4</f>
         <v>1192</v>
       </c>
-      <c r="K4" s="24">
+      <c r="K4" s="19">
         <v>0.7</v>
       </c>
-      <c r="L4" s="25">
+      <c r="L4" s="20">
         <f>H4/K4</f>
         <v>1242.8571428571429</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="26">
-        <f>F4</f>
+      <c r="D5" s="21">
+        <f t="shared" ref="D5:E8" si="0">F4</f>
         <v>870</v>
       </c>
-      <c r="E5" s="27">
-        <f>G4</f>
+      <c r="E5" s="22">
+        <f t="shared" si="0"/>
         <v>1272</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="23">
         <v>2471140</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="24">
         <v>2817150</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="14">
         <f>F5-D5</f>
         <v>2470270</v>
       </c>
-      <c r="I5" s="23">
+      <c r="I5" s="18">
         <f>J5-H5</f>
         <v>345608</v>
       </c>
-      <c r="J5" s="20">
+      <c r="J5" s="15">
         <f>G5-E5</f>
         <v>2815878</v>
       </c>
-      <c r="K5" s="24">
+      <c r="K5" s="19">
         <v>54.6</v>
       </c>
-      <c r="L5" s="25">
-        <f t="shared" ref="L5:L7" si="0">H5/K5</f>
+      <c r="L5" s="20">
+        <f t="shared" ref="L5:L7" si="1">H5/K5</f>
         <v>45243.040293040292</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="26">
-        <f>F5</f>
+      <c r="D6" s="21">
+        <f t="shared" si="0"/>
         <v>2471140</v>
       </c>
-      <c r="E6" s="27">
-        <f>G5</f>
+      <c r="E6" s="22">
+        <f t="shared" si="0"/>
         <v>2817150</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="23">
         <v>2668941</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="24">
         <v>3038593</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="14">
         <f>F6-D6</f>
         <v>197801</v>
       </c>
-      <c r="I6" s="23">
+      <c r="I6" s="18">
         <f>J6-H6</f>
         <v>23642</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="15">
         <f>G6-E6</f>
         <v>221443</v>
       </c>
-      <c r="K6" s="24">
+      <c r="K6" s="19">
         <v>4.5999999999999996</v>
       </c>
-      <c r="L6" s="25">
-        <f t="shared" si="0"/>
+      <c r="L6" s="20">
+        <f t="shared" si="1"/>
         <v>43000.217391304352</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="26">
-        <f>F6</f>
+      <c r="D7" s="21">
+        <f t="shared" si="0"/>
         <v>2668941</v>
       </c>
-      <c r="E7" s="27">
-        <f>G6</f>
+      <c r="E7" s="22">
+        <f t="shared" si="0"/>
         <v>3038593</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="14">
         <v>7902266</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="24">
         <v>8591092</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="14">
         <f>F7-D7</f>
         <v>5233325</v>
       </c>
-      <c r="I7" s="23">
+      <c r="I7" s="18">
         <f>J7-H7</f>
         <v>319174</v>
       </c>
-      <c r="J7" s="20">
+      <c r="J7" s="15">
         <f>G7-E7</f>
         <v>5552499</v>
       </c>
-      <c r="K7" s="24">
+      <c r="K7" s="19">
         <v>126.3</v>
       </c>
-      <c r="L7" s="25">
-        <f t="shared" si="0"/>
+      <c r="L7" s="20">
+        <f t="shared" si="1"/>
         <v>41435.669041963578</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="26">
-        <f>F7</f>
+      <c r="D8" s="21">
+        <f t="shared" si="0"/>
         <v>7902266</v>
       </c>
-      <c r="E8" s="27">
-        <f>G7</f>
+      <c r="E8" s="22">
+        <f t="shared" si="0"/>
         <v>8591092</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="23">
         <v>12981450</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="24">
         <v>13670282</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="14">
         <f>F8-D8</f>
         <v>5079184</v>
       </c>
-      <c r="I8" s="23">
+      <c r="I8" s="18">
         <f>J8-H8</f>
         <v>6</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="15">
         <f>G8-E8</f>
         <v>5079190</v>
       </c>
-      <c r="K8" s="24">
+      <c r="K8" s="19">
         <v>123.6</v>
       </c>
-      <c r="L8" s="25">
-        <f t="shared" ref="L8" si="1">H8/K8</f>
+      <c r="L8" s="20">
+        <f t="shared" ref="L8" si="2">H8/K8</f>
         <v>41093.7216828479</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="26">
-        <f t="shared" ref="D9" si="2">F8</f>
+      <c r="D9" s="21">
+        <f t="shared" ref="D9" si="3">F8</f>
         <v>12981450</v>
       </c>
-      <c r="E9" s="27">
-        <f t="shared" ref="E9" si="3">G8</f>
+      <c r="E9" s="22">
+        <f t="shared" ref="E9" si="4">G8</f>
         <v>13670282</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="23">
         <v>14937999</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="24">
         <v>15626835</v>
       </c>
-      <c r="H9" s="19">
-        <f t="shared" ref="H9:H15" si="4">F9-D9</f>
+      <c r="H9" s="14">
+        <f t="shared" ref="H9:H15" si="5">F9-D9</f>
         <v>1956549</v>
       </c>
-      <c r="I9" s="23">
-        <f t="shared" ref="I9:I15" si="5">J9-H9</f>
+      <c r="I9" s="18">
+        <f t="shared" ref="I9:I15" si="6">J9-H9</f>
         <v>4</v>
       </c>
-      <c r="J9" s="20">
-        <f t="shared" ref="J9:J15" si="6">G9-E9</f>
+      <c r="J9" s="15">
+        <f t="shared" ref="J9:J15" si="7">G9-E9</f>
         <v>1956553</v>
       </c>
-      <c r="K9" s="24">
+      <c r="K9" s="19">
         <v>49.5</v>
       </c>
-      <c r="L9" s="25">
-        <f t="shared" ref="L9:L15" si="7">H9/K9</f>
+      <c r="L9" s="20">
+        <f t="shared" ref="L9:L15" si="8">H9/K9</f>
         <v>39526.242424242424</v>
       </c>
-      <c r="M9" s="30">
+      <c r="M9" s="25">
         <v>1956549</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="25"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="20"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="25"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="20"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="26">
+      <c r="D12" s="21">
         <f>F9</f>
         <v>14937999</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="22">
         <f>G9</f>
         <v>15626835</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="23">
         <v>14939032</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G12" s="24">
         <v>15628207</v>
       </c>
-      <c r="H12" s="19">
-        <f t="shared" si="4"/>
+      <c r="H12" s="14">
+        <f t="shared" si="5"/>
         <v>1033</v>
       </c>
-      <c r="I12" s="23">
-        <f t="shared" si="5"/>
+      <c r="I12" s="18">
+        <f t="shared" si="6"/>
         <v>339</v>
       </c>
-      <c r="J12" s="20">
-        <f t="shared" si="6"/>
+      <c r="J12" s="15">
+        <f t="shared" si="7"/>
         <v>1372</v>
       </c>
-      <c r="K12" s="24">
+      <c r="K12" s="19">
         <v>0.2</v>
       </c>
-      <c r="L12" s="25">
-        <f t="shared" si="7"/>
+      <c r="L12" s="20">
+        <f t="shared" si="8"/>
         <v>5165</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="55" t="s">
+      <c r="C13" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="21">
         <f>F12</f>
         <v>14939032</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="22">
         <f>G12</f>
         <v>15628207</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="23">
         <v>15579732</v>
       </c>
-      <c r="G13" s="29">
+      <c r="G13" s="24">
         <v>16590188</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="14">
         <f>F13-D13</f>
         <v>640700</v>
       </c>
-      <c r="I13" s="23">
+      <c r="I13" s="18">
         <f>J13-H13</f>
         <v>321281</v>
       </c>
-      <c r="J13" s="20">
+      <c r="J13" s="15">
         <f>G13-E13</f>
         <v>961981</v>
       </c>
-      <c r="K13" s="24">
+      <c r="K13" s="19">
         <v>136.4</v>
       </c>
-      <c r="L13" s="25">
+      <c r="L13" s="20">
         <f>H13/K13</f>
         <v>4697.2140762463341</v>
       </c>
-      <c r="M13" s="30">
+      <c r="M13" s="25">
         <f>640700</f>
         <v>640700</v>
       </c>
@@ -1804,132 +1833,132 @@
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="26">
-        <f t="shared" ref="D14:D16" si="8">F13</f>
+      <c r="D14" s="21">
+        <f t="shared" ref="D14:D16" si="9">F13</f>
         <v>15579732</v>
       </c>
-      <c r="E14" s="27">
-        <f t="shared" ref="E14:E16" si="9">G13</f>
+      <c r="E14" s="22">
+        <f t="shared" ref="E14:E16" si="10">G13</f>
         <v>16590188</v>
       </c>
-      <c r="F14" s="28">
+      <c r="F14" s="23">
         <v>16142326</v>
       </c>
-      <c r="G14" s="29">
+      <c r="G14" s="24">
         <v>17235242</v>
       </c>
-      <c r="H14" s="19">
-        <f t="shared" si="4"/>
+      <c r="H14" s="14">
+        <f t="shared" si="5"/>
         <v>562594</v>
       </c>
-      <c r="I14" s="23">
-        <f t="shared" si="5"/>
+      <c r="I14" s="18">
+        <f t="shared" si="6"/>
         <v>82460</v>
       </c>
-      <c r="J14" s="20">
-        <f t="shared" si="6"/>
+      <c r="J14" s="15">
+        <f t="shared" si="7"/>
         <v>645054</v>
       </c>
-      <c r="K14" s="24">
+      <c r="K14" s="19">
         <v>18.899999999999999</v>
       </c>
-      <c r="L14" s="25">
-        <f t="shared" si="7"/>
+      <c r="L14" s="20">
+        <f t="shared" si="8"/>
         <v>29766.878306878309</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="21">
+        <f t="shared" si="9"/>
+        <v>16142326</v>
+      </c>
+      <c r="E15" s="22">
+        <f t="shared" si="10"/>
+        <v>17235242</v>
+      </c>
+      <c r="F15" s="23">
+        <v>17147475</v>
+      </c>
+      <c r="G15" s="24">
+        <v>19758781</v>
+      </c>
+      <c r="H15" s="14">
+        <f t="shared" si="5"/>
+        <v>1005149</v>
+      </c>
+      <c r="I15" s="18">
+        <f t="shared" si="6"/>
+        <v>1518390</v>
+      </c>
+      <c r="J15" s="15">
+        <f t="shared" si="7"/>
+        <v>2523539</v>
+      </c>
+      <c r="K15" s="19">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="L15" s="20">
         <f t="shared" si="8"/>
-        <v>16142326</v>
-      </c>
-      <c r="E15" s="27">
-        <f t="shared" si="9"/>
-        <v>17235242</v>
-      </c>
-      <c r="F15" s="28">
-        <v>17147475</v>
-      </c>
-      <c r="G15" s="29">
-        <v>19758781</v>
-      </c>
-      <c r="H15" s="19">
-        <f t="shared" si="4"/>
-        <v>1005149</v>
-      </c>
-      <c r="I15" s="23">
-        <f t="shared" si="5"/>
-        <v>1518390</v>
-      </c>
-      <c r="J15" s="20">
-        <f t="shared" si="6"/>
-        <v>2523539</v>
-      </c>
-      <c r="K15" s="24">
-        <v>67.099999999999994</v>
-      </c>
-      <c r="L15" s="25">
-        <f t="shared" si="7"/>
         <v>14979.865871833086</v>
       </c>
-      <c r="M15" s="30">
+      <c r="M15" s="25">
         <f>1004149</f>
         <v>1004149</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="26">
-        <f t="shared" si="8"/>
+      <c r="D16" s="21">
+        <f t="shared" si="9"/>
         <v>17147475</v>
       </c>
-      <c r="E16" s="27">
-        <f t="shared" si="9"/>
+      <c r="E16" s="22">
+        <f t="shared" si="10"/>
         <v>19758781</v>
       </c>
-      <c r="F16" s="28">
+      <c r="F16" s="23">
         <v>17466625</v>
       </c>
-      <c r="G16" s="28">
+      <c r="G16" s="23">
         <v>20077933</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="14">
         <f>F16-D16</f>
         <v>319150</v>
       </c>
-      <c r="I16" s="23">
+      <c r="I16" s="18">
         <f>J16-H16</f>
         <v>2</v>
       </c>
-      <c r="J16" s="20">
+      <c r="J16" s="15">
         <f>G16-E16</f>
         <v>319152</v>
       </c>
-      <c r="K16" s="24">
+      <c r="K16" s="19">
         <v>136.4</v>
       </c>
-      <c r="L16" s="25">
+      <c r="L16" s="20">
         <f>H16/K16</f>
         <v>2339.8093841642226</v>
       </c>
-      <c r="M16" s="30">
+      <c r="M16" s="25">
         <f>319150</f>
         <v>319150</v>
       </c>
@@ -1938,265 +1967,284 @@
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="26">
-        <f t="shared" ref="D17" si="10">F16</f>
+      <c r="D17" s="21">
+        <f t="shared" ref="D17" si="11">F16</f>
         <v>17466625</v>
       </c>
-      <c r="E17" s="27">
-        <f t="shared" ref="E17" si="11">G16</f>
+      <c r="E17" s="22">
+        <f t="shared" ref="E17" si="12">G16</f>
         <v>20077933</v>
       </c>
-      <c r="F17" s="28">
+      <c r="F17" s="23">
         <v>17466877</v>
       </c>
-      <c r="G17" s="28">
+      <c r="G17" s="23">
         <v>20078985</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="14">
         <f>F17-D17</f>
         <v>252</v>
       </c>
-      <c r="I17" s="23">
+      <c r="I17" s="18">
         <f>J17-H17</f>
         <v>800</v>
       </c>
-      <c r="J17" s="20">
+      <c r="J17" s="15">
         <f>G17-E17</f>
         <v>1052</v>
       </c>
-      <c r="K17" s="24">
+      <c r="K17" s="19">
         <v>0.1</v>
       </c>
-      <c r="L17" s="25">
+      <c r="L17" s="20">
         <f>H17/K17</f>
         <v>2520</v>
       </c>
-      <c r="M17" s="30"/>
+      <c r="M17" s="25"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="54" t="s">
+      <c r="B18" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="26">
-        <f t="shared" ref="D18:D20" si="12">F17</f>
+      <c r="D18" s="21">
+        <f t="shared" ref="D18:D20" si="13">F17</f>
         <v>17466877</v>
       </c>
-      <c r="E18" s="27">
-        <f t="shared" ref="E18:E20" si="13">G17</f>
+      <c r="E18" s="22">
+        <f t="shared" ref="E18:E20" si="14">G17</f>
         <v>20078985</v>
       </c>
-      <c r="F18" s="28">
+      <c r="F18" s="23">
         <v>18432297</v>
       </c>
-      <c r="G18" s="28">
+      <c r="G18" s="23">
         <v>21169222</v>
       </c>
-      <c r="H18" s="19">
+      <c r="H18" s="14">
         <f>F18-D18</f>
         <v>965420</v>
       </c>
-      <c r="I18" s="23">
+      <c r="I18" s="18">
         <f>J18-H18</f>
         <v>124817</v>
       </c>
-      <c r="J18" s="20">
+      <c r="J18" s="15">
         <f>G18-E18</f>
         <v>1090237</v>
       </c>
-      <c r="K18" s="24">
+      <c r="K18" s="19">
         <v>31.3</v>
       </c>
-      <c r="L18" s="25">
+      <c r="L18" s="20">
         <f>H18/K18</f>
         <v>30844.089456869009</v>
       </c>
-      <c r="M18" s="30"/>
+      <c r="M18" s="25"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="54" t="s">
+      <c r="B19" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="26">
-        <f t="shared" si="12"/>
+      <c r="D19" s="21">
+        <f t="shared" si="13"/>
         <v>18432297</v>
       </c>
-      <c r="E19" s="27">
-        <f t="shared" si="13"/>
+      <c r="E19" s="22">
+        <f t="shared" si="14"/>
         <v>21169222</v>
       </c>
-      <c r="F19" s="28">
+      <c r="F19" s="23">
         <v>18831233</v>
       </c>
-      <c r="G19" s="29">
+      <c r="G19" s="24">
         <v>21568158</v>
       </c>
-      <c r="H19" s="19">
-        <f t="shared" ref="H19:H20" si="14">F19-D19</f>
+      <c r="H19" s="14">
+        <f t="shared" ref="H19:H20" si="15">F19-D19</f>
         <v>398936</v>
       </c>
-      <c r="I19" s="23">
-        <f t="shared" ref="I19:I20" si="15">J19-H19</f>
+      <c r="I19" s="18">
+        <f t="shared" ref="I19:I20" si="16">J19-H19</f>
         <v>0</v>
       </c>
-      <c r="J19" s="20">
-        <f t="shared" ref="J19:J20" si="16">G19-E19</f>
+      <c r="J19" s="15">
+        <f t="shared" ref="J19:J20" si="17">G19-E19</f>
         <v>398936</v>
       </c>
-      <c r="K19" s="24">
+      <c r="K19" s="19">
         <v>28.5</v>
       </c>
-      <c r="L19" s="25">
-        <f t="shared" ref="L19:L20" si="17">H19/K19</f>
+      <c r="L19" s="20">
+        <f t="shared" ref="L19:L20" si="18">H19/K19</f>
         <v>13997.754385964912</v>
       </c>
-      <c r="M19" s="30">
+      <c r="M19" s="25">
         <v>398936</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="54" t="s">
+      <c r="B20" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="26">
-        <f t="shared" si="12"/>
+      <c r="D20" s="21">
+        <f t="shared" si="13"/>
         <v>18831233</v>
       </c>
-      <c r="E20" s="27">
-        <f t="shared" si="13"/>
+      <c r="E20" s="22">
+        <f t="shared" si="14"/>
         <v>21568158</v>
       </c>
-      <c r="F20" s="28">
+      <c r="F20" s="23">
         <v>19031024</v>
       </c>
-      <c r="G20" s="29">
+      <c r="G20" s="24">
         <v>21769051</v>
       </c>
-      <c r="H20" s="19">
-        <f t="shared" si="14"/>
+      <c r="H20" s="14">
+        <f t="shared" si="15"/>
         <v>199791</v>
       </c>
-      <c r="I20" s="23">
-        <f t="shared" si="15"/>
+      <c r="I20" s="18">
+        <f t="shared" si="16"/>
         <v>1102</v>
       </c>
-      <c r="J20" s="20">
-        <f t="shared" si="16"/>
+      <c r="J20" s="15">
+        <f t="shared" si="17"/>
         <v>200893</v>
       </c>
-      <c r="K20" s="24">
+      <c r="K20" s="19">
         <v>18.100000000000001</v>
       </c>
-      <c r="L20" s="25">
-        <f t="shared" si="17"/>
+      <c r="L20" s="20">
+        <f t="shared" si="18"/>
         <v>11038.17679558011</v>
       </c>
-      <c r="M20" s="30">
+      <c r="M20" s="25">
         <v>199791</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B21" s="54" t="s">
+      <c r="B21" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="55" t="s">
+      <c r="C21" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="26">
+      <c r="D21" s="21">
         <f>F20</f>
         <v>19031024</v>
       </c>
-      <c r="E21" s="27">
+      <c r="E21" s="22">
         <f>G20</f>
         <v>21769051</v>
       </c>
-      <c r="F21" s="28">
+      <c r="F21" s="23">
         <v>19154932</v>
       </c>
-      <c r="G21" s="29">
+      <c r="G21" s="24">
         <v>21956551</v>
       </c>
-      <c r="H21" s="19">
+      <c r="H21" s="14">
         <f>F21-D21</f>
         <v>123908</v>
       </c>
-      <c r="I21" s="23">
+      <c r="I21" s="18">
         <f>J21-H21</f>
         <v>63592</v>
       </c>
-      <c r="J21" s="20">
+      <c r="J21" s="15">
         <f>G21-E21</f>
         <v>187500</v>
       </c>
-      <c r="K21" s="24">
+      <c r="K21" s="19">
         <v>153</v>
       </c>
-      <c r="L21" s="25">
+      <c r="L21" s="20">
         <f>H21/K21</f>
         <v>809.85620915032678</v>
       </c>
-      <c r="M21" s="30">
+      <c r="M21" s="25">
         <v>123908</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="32"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="30"/>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B22" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="15"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="20"/>
     </row>
-    <row r="23" spans="2:14" s="51" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="43" t="s">
+    <row r="23" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="27"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="25"/>
+    </row>
+    <row r="24" spans="2:14" s="46" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="44"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="45">
-        <f>SUM(H4:H22)+D4</f>
+      <c r="C24" s="39"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="40">
+        <f>SUM(H4:H23)+D4</f>
         <v>19154932</v>
       </c>
-      <c r="I23" s="49">
-        <f>SUM(I4:I22)+(E4-D4)</f>
+      <c r="I24" s="44">
+        <f>SUM(I4:I23)+(E4-D4)</f>
         <v>2801619</v>
       </c>
-      <c r="J23" s="46">
-        <f>SUM(J4:J22)+E4</f>
+      <c r="J24" s="41">
+        <f>SUM(J4:J23)+E4</f>
         <v>21956551</v>
       </c>
-      <c r="K23" s="43">
-        <f>SUM(K4:K22)</f>
+      <c r="K24" s="38">
+        <f>SUM(K4:K23)</f>
         <v>949.3</v>
       </c>
-      <c r="L23" s="50">
-        <f>H23/K23</f>
+      <c r="L24" s="45">
+        <f>H24/K24</f>
         <v>20177.954282102604</v>
       </c>
     </row>
@@ -2216,9 +2264,10 @@
     <hyperlink ref="C17" r:id="rId7" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
     <hyperlink ref="C18" r:id="rId8" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
     <hyperlink ref="C21" r:id="rId9" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
+    <hyperlink ref="C22" r:id="rId10" display="http://data.ontotext.com/resource/leaks/ontology"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967294" r:id="rId10"/>
-  <legacyDrawing r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967294" r:id="rId11"/>
+  <legacyDrawing r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
after the second load
</commit_message>
<xml_diff>
--- a/leaks-load.xlsx
+++ b/leaks-load.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="First load" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -232,7 +233,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="53">
   <si>
     <t>file</t>
   </si>
@@ -367,6 +368,30 @@
   </si>
   <si>
     <t>….</t>
+  </si>
+  <si>
+    <t>INSERT: see-also.ru</t>
+  </si>
+  <si>
+    <t>leaks:see-also</t>
+  </si>
+  <si>
+    <t>BEFORE</t>
+  </si>
+  <si>
+    <t>AFTER</t>
+  </si>
+  <si>
+    <t>DIFF</t>
+  </si>
+  <si>
+    <t>leaks:country-external-schema</t>
+  </si>
+  <si>
+    <t>geonames_ontology_v3.1-leaks.ttl</t>
+  </si>
+  <si>
+    <t>dbpedia-geonames-countries.ttl</t>
   </si>
 </sst>
 </file>
@@ -1000,7 +1025,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1067,6 +1092,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1371,11 +1400,890 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="1.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="52"/>
+      <c r="F2" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="54"/>
+      <c r="H2" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="55"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="48" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B4" s="57" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0</v>
+      </c>
+      <c r="E4" s="15">
+        <v>80</v>
+      </c>
+      <c r="F4" s="16">
+        <v>252</v>
+      </c>
+      <c r="G4" s="17">
+        <v>517</v>
+      </c>
+      <c r="H4" s="14">
+        <f>F4-D4</f>
+        <v>252</v>
+      </c>
+      <c r="I4" s="18">
+        <f>J4-H4</f>
+        <v>185</v>
+      </c>
+      <c r="J4" s="15">
+        <f>G4-E4</f>
+        <v>437</v>
+      </c>
+      <c r="K4" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="L4" s="20">
+        <f>H4/K4</f>
+        <v>2520</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="21">
+        <f>F4</f>
+        <v>252</v>
+      </c>
+      <c r="E5" s="22">
+        <f>G4</f>
+        <v>517</v>
+      </c>
+      <c r="F5" s="23">
+        <v>1126</v>
+      </c>
+      <c r="G5" s="23">
+        <v>1727</v>
+      </c>
+      <c r="H5" s="14">
+        <f>F5-D5</f>
+        <v>874</v>
+      </c>
+      <c r="I5" s="18">
+        <f>J5-H5</f>
+        <v>336</v>
+      </c>
+      <c r="J5" s="15">
+        <f>G5-E5</f>
+        <v>1210</v>
+      </c>
+      <c r="K5" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="L5" s="20">
+        <f>H5/K5</f>
+        <v>8740</v>
+      </c>
+      <c r="M5" s="25"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="21">
+        <f t="shared" ref="D6:D18" si="0">F5</f>
+        <v>1126</v>
+      </c>
+      <c r="E6" s="22">
+        <f t="shared" ref="E6:E18" si="1">G5</f>
+        <v>1727</v>
+      </c>
+      <c r="F6" s="23">
+        <v>2471396</v>
+      </c>
+      <c r="G6" s="23">
+        <v>2817605</v>
+      </c>
+      <c r="H6" s="14">
+        <f t="shared" ref="H6:H20" si="2">F6-D6</f>
+        <v>2470270</v>
+      </c>
+      <c r="I6" s="18">
+        <f t="shared" ref="I6:I20" si="3">J6-H6</f>
+        <v>345608</v>
+      </c>
+      <c r="J6" s="15">
+        <f t="shared" ref="J6:J20" si="4">G6-E6</f>
+        <v>2815878</v>
+      </c>
+      <c r="K6" s="19">
+        <v>62.2</v>
+      </c>
+      <c r="L6" s="20">
+        <f t="shared" ref="L6:L20" si="5">H6/K6</f>
+        <v>39714.951768488747</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="21">
+        <f t="shared" si="0"/>
+        <v>2471396</v>
+      </c>
+      <c r="E7" s="22">
+        <f t="shared" si="1"/>
+        <v>2817605</v>
+      </c>
+      <c r="F7" s="23">
+        <v>2669197</v>
+      </c>
+      <c r="G7" s="23">
+        <v>3039048</v>
+      </c>
+      <c r="H7" s="14">
+        <f t="shared" si="2"/>
+        <v>197801</v>
+      </c>
+      <c r="I7" s="18">
+        <f t="shared" si="3"/>
+        <v>23642</v>
+      </c>
+      <c r="J7" s="15">
+        <f t="shared" si="4"/>
+        <v>221443</v>
+      </c>
+      <c r="K7" s="19">
+        <v>5.3</v>
+      </c>
+      <c r="L7" s="20">
+        <f t="shared" si="5"/>
+        <v>37320.943396226416</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B8" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="21">
+        <f t="shared" si="0"/>
+        <v>2669197</v>
+      </c>
+      <c r="E8" s="22">
+        <f t="shared" si="1"/>
+        <v>3039048</v>
+      </c>
+      <c r="F8" s="23">
+        <v>7902522</v>
+      </c>
+      <c r="G8" s="23">
+        <v>8591547</v>
+      </c>
+      <c r="H8" s="14">
+        <f t="shared" si="2"/>
+        <v>5233325</v>
+      </c>
+      <c r="I8" s="18">
+        <f t="shared" si="3"/>
+        <v>319174</v>
+      </c>
+      <c r="J8" s="15">
+        <f t="shared" si="4"/>
+        <v>5552499</v>
+      </c>
+      <c r="K8" s="19">
+        <v>139.5</v>
+      </c>
+      <c r="L8" s="20">
+        <f t="shared" si="5"/>
+        <v>37514.874551971327</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="21">
+        <f t="shared" si="0"/>
+        <v>7902522</v>
+      </c>
+      <c r="E9" s="22">
+        <f t="shared" si="1"/>
+        <v>8591547</v>
+      </c>
+      <c r="F9" s="23">
+        <v>12981706</v>
+      </c>
+      <c r="G9" s="23">
+        <v>13670737</v>
+      </c>
+      <c r="H9" s="14">
+        <f t="shared" si="2"/>
+        <v>5079184</v>
+      </c>
+      <c r="I9" s="18">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="J9" s="15">
+        <f t="shared" si="4"/>
+        <v>5079190</v>
+      </c>
+      <c r="K9" s="19">
+        <v>137.80000000000001</v>
+      </c>
+      <c r="L9" s="20">
+        <f t="shared" si="5"/>
+        <v>36859.100145137876</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B10" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="21">
+        <f t="shared" si="0"/>
+        <v>12981706</v>
+      </c>
+      <c r="E10" s="22">
+        <f t="shared" si="1"/>
+        <v>13670737</v>
+      </c>
+      <c r="F10" s="23">
+        <v>13947126</v>
+      </c>
+      <c r="G10" s="23">
+        <v>14760974</v>
+      </c>
+      <c r="H10" s="14">
+        <f t="shared" si="2"/>
+        <v>965420</v>
+      </c>
+      <c r="I10" s="18">
+        <f t="shared" si="3"/>
+        <v>124817</v>
+      </c>
+      <c r="J10" s="15">
+        <f t="shared" si="4"/>
+        <v>1090237</v>
+      </c>
+      <c r="K10" s="19">
+        <v>25.8</v>
+      </c>
+      <c r="L10" s="20">
+        <f t="shared" si="5"/>
+        <v>37419.379844961237</v>
+      </c>
+      <c r="M10" s="25"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B11" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="21">
+        <f t="shared" si="0"/>
+        <v>13947126</v>
+      </c>
+      <c r="E11" s="22">
+        <f t="shared" si="1"/>
+        <v>14760974</v>
+      </c>
+      <c r="F11" s="23">
+        <v>14760317</v>
+      </c>
+      <c r="G11" s="23">
+        <v>15574165</v>
+      </c>
+      <c r="H11" s="14">
+        <f t="shared" si="2"/>
+        <v>813191</v>
+      </c>
+      <c r="I11" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="15">
+        <f t="shared" si="4"/>
+        <v>813191</v>
+      </c>
+      <c r="K11" s="19">
+        <v>31.4</v>
+      </c>
+      <c r="L11" s="20">
+        <f t="shared" si="5"/>
+        <v>25897.802547770701</v>
+      </c>
+      <c r="M11" s="25">
+        <v>813191</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="21">
+        <f t="shared" si="0"/>
+        <v>14760317</v>
+      </c>
+      <c r="E12" s="22">
+        <f t="shared" si="1"/>
+        <v>15574165</v>
+      </c>
+      <c r="F12" s="23">
+        <v>17115802</v>
+      </c>
+      <c r="G12" s="23">
+        <v>17929654</v>
+      </c>
+      <c r="H12" s="14">
+        <f t="shared" si="2"/>
+        <v>2355485</v>
+      </c>
+      <c r="I12" s="18">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="J12" s="15">
+        <f t="shared" si="4"/>
+        <v>2355489</v>
+      </c>
+      <c r="K12" s="19">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="L12" s="20">
+        <f t="shared" si="5"/>
+        <v>36575.854037267076</v>
+      </c>
+      <c r="M12" s="25">
+        <v>2355485</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B13" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="15">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="19"/>
+      <c r="L13" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B14" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="15">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="19"/>
+      <c r="L14" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="21">
+        <f>F12</f>
+        <v>17115802</v>
+      </c>
+      <c r="E15" s="22">
+        <f>G12</f>
+        <v>17929654</v>
+      </c>
+      <c r="F15" s="23">
+        <v>17116835</v>
+      </c>
+      <c r="G15" s="23">
+        <v>17931652</v>
+      </c>
+      <c r="H15" s="14">
+        <f t="shared" si="2"/>
+        <v>1033</v>
+      </c>
+      <c r="I15" s="18">
+        <f t="shared" si="3"/>
+        <v>965</v>
+      </c>
+      <c r="J15" s="15">
+        <f t="shared" si="4"/>
+        <v>1998</v>
+      </c>
+      <c r="K15" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="L15" s="20">
+        <f t="shared" si="5"/>
+        <v>10330</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B16" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="21">
+        <f t="shared" si="0"/>
+        <v>17116835</v>
+      </c>
+      <c r="E16" s="22">
+        <f t="shared" si="1"/>
+        <v>17931652</v>
+      </c>
+      <c r="F16" s="23">
+        <v>17881443</v>
+      </c>
+      <c r="G16" s="23">
+        <v>19080905</v>
+      </c>
+      <c r="H16" s="14">
+        <f t="shared" si="2"/>
+        <v>764608</v>
+      </c>
+      <c r="I16" s="18">
+        <f t="shared" si="3"/>
+        <v>384645</v>
+      </c>
+      <c r="J16" s="15">
+        <f t="shared" si="4"/>
+        <v>1149253</v>
+      </c>
+      <c r="K16" s="19">
+        <v>172.7</v>
+      </c>
+      <c r="L16" s="20">
+        <f t="shared" si="5"/>
+        <v>4427.3769542559357</v>
+      </c>
+      <c r="M16" s="25">
+        <v>764608</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B17" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="21">
+        <f t="shared" si="0"/>
+        <v>17881443</v>
+      </c>
+      <c r="E17" s="22">
+        <f t="shared" si="1"/>
+        <v>19080905</v>
+      </c>
+      <c r="F17" s="23">
+        <v>18200593</v>
+      </c>
+      <c r="G17" s="23">
+        <v>19400057</v>
+      </c>
+      <c r="H17" s="14">
+        <f t="shared" si="2"/>
+        <v>319150</v>
+      </c>
+      <c r="I17" s="18">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J17" s="15">
+        <f t="shared" si="4"/>
+        <v>319152</v>
+      </c>
+      <c r="K17" s="19">
+        <v>6.9</v>
+      </c>
+      <c r="L17" s="20">
+        <f t="shared" si="5"/>
+        <v>46253.623188405792</v>
+      </c>
+      <c r="M17" s="25">
+        <v>319150</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B18" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="21">
+        <f t="shared" si="0"/>
+        <v>18200593</v>
+      </c>
+      <c r="E18" s="22">
+        <f t="shared" si="1"/>
+        <v>19400057</v>
+      </c>
+      <c r="F18" s="23">
+        <v>19404533</v>
+      </c>
+      <c r="G18" s="23">
+        <v>22533290</v>
+      </c>
+      <c r="H18" s="14">
+        <f t="shared" si="2"/>
+        <v>1203940</v>
+      </c>
+      <c r="I18" s="18">
+        <f t="shared" si="3"/>
+        <v>1929293</v>
+      </c>
+      <c r="J18" s="15">
+        <f t="shared" si="4"/>
+        <v>3133233</v>
+      </c>
+      <c r="K18" s="19">
+        <v>85.9</v>
+      </c>
+      <c r="L18" s="20">
+        <f t="shared" si="5"/>
+        <v>14015.599534342258</v>
+      </c>
+      <c r="M18" s="25">
+        <v>1203940</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B19" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="21">
+        <f t="shared" ref="D19" si="6">F18</f>
+        <v>19404533</v>
+      </c>
+      <c r="E19" s="22">
+        <f t="shared" ref="E19" si="7">G18</f>
+        <v>22533290</v>
+      </c>
+      <c r="F19" s="23">
+        <v>19411294</v>
+      </c>
+      <c r="G19" s="23">
+        <v>22544573</v>
+      </c>
+      <c r="H19" s="14">
+        <f t="shared" ref="H19" si="8">F19-D19</f>
+        <v>6761</v>
+      </c>
+      <c r="I19" s="18">
+        <f t="shared" si="3"/>
+        <v>4522</v>
+      </c>
+      <c r="J19" s="15">
+        <f t="shared" ref="J19" si="9">G19-E19</f>
+        <v>11283</v>
+      </c>
+      <c r="K19" s="19">
+        <v>0.4</v>
+      </c>
+      <c r="L19" s="20">
+        <f t="shared" ref="L19" si="10">H19/K19</f>
+        <v>16902.5</v>
+      </c>
+      <c r="M19" s="25">
+        <v>1203940</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B20" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="21">
+        <f>F18</f>
+        <v>19404533</v>
+      </c>
+      <c r="E20" s="22">
+        <f>G18</f>
+        <v>22533290</v>
+      </c>
+      <c r="F20" s="23">
+        <v>19414136</v>
+      </c>
+      <c r="G20" s="23">
+        <v>22550031</v>
+      </c>
+      <c r="H20" s="14">
+        <f t="shared" si="2"/>
+        <v>9603</v>
+      </c>
+      <c r="I20" s="18">
+        <f t="shared" si="3"/>
+        <v>7138</v>
+      </c>
+      <c r="J20" s="15">
+        <f t="shared" si="4"/>
+        <v>16741</v>
+      </c>
+      <c r="K20" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="L20" s="20">
+        <f t="shared" si="5"/>
+        <v>48015</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="27"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="25"/>
+    </row>
+    <row r="22" spans="2:14" s="46" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="39"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="40">
+        <f>SUM(H4:H21)+D4</f>
+        <v>19420897</v>
+      </c>
+      <c r="I22" s="44">
+        <f>SUM(I4:I21)+(E4-D4)</f>
+        <v>3140417</v>
+      </c>
+      <c r="J22" s="41">
+        <f>SUM(J4:J21)+E4</f>
+        <v>22561314</v>
+      </c>
+      <c r="K22" s="38">
+        <f>SUM(K4:K21)</f>
+        <v>732.80000000000007</v>
+      </c>
+      <c r="L22" s="45">
+        <f>H22/K22</f>
+        <v>26502.315775109168</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B25" s="56"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B26" s="56"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="59"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B27" s="56"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:J2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C6" r:id="rId1" display="http://data.ontotext.com/resource/leaks/raw-data"/>
+    <hyperlink ref="C13" r:id="rId2" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
+    <hyperlink ref="C7:C9" r:id="rId3" display="http://data.ontotext.com/resource/leaks/raw-data"/>
+    <hyperlink ref="C17" r:id="rId4" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
+    <hyperlink ref="C10" r:id="rId5" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
+    <hyperlink ref="C11" r:id="rId6" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
+    <hyperlink ref="C5" r:id="rId7" display="http://data.ontotext.com/resource/leaks/ontology"/>
+    <hyperlink ref="C4" r:id="rId8" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
+    <hyperlink ref="C19" r:id="rId9" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967294" r:id="rId10"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:N25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1509,7 +2417,7 @@
         <v>21</v>
       </c>
       <c r="D5" s="21">
-        <f t="shared" ref="D5:E8" si="0">F4</f>
+        <f t="shared" ref="D5:E9" si="0">F4</f>
         <v>870</v>
       </c>
       <c r="E5" s="22">
@@ -1538,7 +2446,7 @@
         <v>54.6</v>
       </c>
       <c r="L5" s="20">
-        <f t="shared" ref="L5:L7" si="1">H5/K5</f>
+        <f t="shared" ref="L5:L15" si="1">H5/K5</f>
         <v>45243.040293040292</v>
       </c>
     </row>
@@ -1661,7 +2569,7 @@
         <v>123.6</v>
       </c>
       <c r="L8" s="20">
-        <f t="shared" ref="L8" si="2">H8/K8</f>
+        <f t="shared" si="1"/>
         <v>41093.7216828479</v>
       </c>
     </row>
@@ -1673,11 +2581,11 @@
         <v>27</v>
       </c>
       <c r="D9" s="21">
-        <f t="shared" ref="D9" si="3">F8</f>
+        <f t="shared" si="0"/>
         <v>12981450</v>
       </c>
       <c r="E9" s="22">
-        <f t="shared" ref="E9" si="4">G8</f>
+        <f t="shared" si="0"/>
         <v>13670282</v>
       </c>
       <c r="F9" s="23">
@@ -1687,22 +2595,22 @@
         <v>15626835</v>
       </c>
       <c r="H9" s="14">
-        <f t="shared" ref="H9:H15" si="5">F9-D9</f>
+        <f t="shared" ref="H9:H15" si="2">F9-D9</f>
         <v>1956549</v>
       </c>
       <c r="I9" s="18">
-        <f t="shared" ref="I9:I15" si="6">J9-H9</f>
+        <f t="shared" ref="I9:I15" si="3">J9-H9</f>
         <v>4</v>
       </c>
       <c r="J9" s="15">
-        <f t="shared" ref="J9:J15" si="7">G9-E9</f>
+        <f t="shared" ref="J9:J15" si="4">G9-E9</f>
         <v>1956553</v>
       </c>
       <c r="K9" s="19">
         <v>49.5</v>
       </c>
       <c r="L9" s="20">
-        <f t="shared" ref="L9:L15" si="8">H9/K9</f>
+        <f t="shared" si="1"/>
         <v>39526.242424242424</v>
       </c>
       <c r="M9" s="25">
@@ -1765,22 +2673,22 @@
         <v>15628207</v>
       </c>
       <c r="H12" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>1033</v>
       </c>
       <c r="I12" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>339</v>
       </c>
       <c r="J12" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>1372</v>
       </c>
       <c r="K12" s="19">
         <v>0.2</v>
       </c>
       <c r="L12" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>5165</v>
       </c>
     </row>
@@ -1840,11 +2748,11 @@
         <v>17</v>
       </c>
       <c r="D14" s="21">
-        <f t="shared" ref="D14:D16" si="9">F13</f>
+        <f t="shared" ref="D14:E20" si="5">F13</f>
         <v>15579732</v>
       </c>
       <c r="E14" s="22">
-        <f t="shared" ref="E14:E16" si="10">G13</f>
+        <f t="shared" si="5"/>
         <v>16590188</v>
       </c>
       <c r="F14" s="23">
@@ -1854,22 +2762,22 @@
         <v>17235242</v>
       </c>
       <c r="H14" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>562594</v>
       </c>
       <c r="I14" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>82460</v>
       </c>
       <c r="J14" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>645054</v>
       </c>
       <c r="K14" s="19">
         <v>18.899999999999999</v>
       </c>
       <c r="L14" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>29766.878306878309</v>
       </c>
     </row>
@@ -1881,11 +2789,11 @@
         <v>33</v>
       </c>
       <c r="D15" s="21">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>16142326</v>
       </c>
       <c r="E15" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>17235242</v>
       </c>
       <c r="F15" s="23">
@@ -1895,22 +2803,22 @@
         <v>19758781</v>
       </c>
       <c r="H15" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>1005149</v>
       </c>
       <c r="I15" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1518390</v>
       </c>
       <c r="J15" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>2523539</v>
       </c>
       <c r="K15" s="19">
         <v>67.099999999999994</v>
       </c>
       <c r="L15" s="20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="1"/>
         <v>14979.865871833086</v>
       </c>
       <c r="M15" s="25">
@@ -1926,11 +2834,11 @@
         <v>39</v>
       </c>
       <c r="D16" s="21">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>17147475</v>
       </c>
       <c r="E16" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>19758781</v>
       </c>
       <c r="F16" s="23">
@@ -1974,11 +2882,11 @@
         <v>41</v>
       </c>
       <c r="D17" s="21">
-        <f t="shared" ref="D17" si="11">F16</f>
+        <f t="shared" si="5"/>
         <v>17466625</v>
       </c>
       <c r="E17" s="22">
-        <f t="shared" ref="E17" si="12">G16</f>
+        <f t="shared" si="5"/>
         <v>20077933</v>
       </c>
       <c r="F17" s="23">
@@ -2016,11 +2924,11 @@
         <v>43</v>
       </c>
       <c r="D18" s="21">
-        <f t="shared" ref="D18:D20" si="13">F17</f>
+        <f t="shared" si="5"/>
         <v>17466877</v>
       </c>
       <c r="E18" s="22">
-        <f t="shared" ref="E18:E20" si="14">G17</f>
+        <f t="shared" si="5"/>
         <v>20078985</v>
       </c>
       <c r="F18" s="23">
@@ -2058,11 +2966,11 @@
         <v>27</v>
       </c>
       <c r="D19" s="21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="5"/>
         <v>18432297</v>
       </c>
       <c r="E19" s="22">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>21169222</v>
       </c>
       <c r="F19" s="23">
@@ -2072,22 +2980,22 @@
         <v>21568158</v>
       </c>
       <c r="H19" s="14">
-        <f t="shared" ref="H19:H20" si="15">F19-D19</f>
+        <f t="shared" ref="H19:H20" si="6">F19-D19</f>
         <v>398936</v>
       </c>
       <c r="I19" s="18">
-        <f t="shared" ref="I19:I20" si="16">J19-H19</f>
+        <f t="shared" ref="I19:I20" si="7">J19-H19</f>
         <v>0</v>
       </c>
       <c r="J19" s="15">
-        <f t="shared" ref="J19:J20" si="17">G19-E19</f>
+        <f t="shared" ref="J19:J20" si="8">G19-E19</f>
         <v>398936</v>
       </c>
       <c r="K19" s="19">
         <v>28.5</v>
       </c>
       <c r="L19" s="20">
-        <f t="shared" ref="L19:L20" si="18">H19/K19</f>
+        <f t="shared" ref="L19:L20" si="9">H19/K19</f>
         <v>13997.754385964912</v>
       </c>
       <c r="M19" s="25">
@@ -2102,11 +3010,11 @@
         <v>33</v>
       </c>
       <c r="D20" s="21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="5"/>
         <v>18831233</v>
       </c>
       <c r="E20" s="22">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>21568158</v>
       </c>
       <c r="F20" s="23">
@@ -2116,22 +3024,22 @@
         <v>21769051</v>
       </c>
       <c r="H20" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>199791</v>
       </c>
       <c r="I20" s="18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>1102</v>
       </c>
       <c r="J20" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>200893</v>
       </c>
       <c r="K20" s="19">
         <v>18.100000000000001</v>
       </c>
       <c r="L20" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>11038.17679558011</v>
       </c>
       <c r="M20" s="25">
@@ -2204,48 +3112,91 @@
       <c r="K22" s="19"/>
       <c r="L22" s="20"/>
     </row>
-    <row r="23" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="27"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="37"/>
-      <c r="M23" s="25"/>
-    </row>
-    <row r="24" spans="2:14" s="46" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="38" t="s">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B23" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="21">
+        <f>F22</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="22">
+        <f>G22</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="23"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="14">
+        <f>F23-D23</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="18">
+        <f>J23-H23</f>
+        <v>0</v>
+      </c>
+      <c r="J23" s="15">
+        <f>G23-E23</f>
+        <v>0</v>
+      </c>
+      <c r="K23" s="19">
+        <v>60</v>
+      </c>
+      <c r="L23" s="20">
+        <f>H23/K23</f>
+        <v>0</v>
+      </c>
+      <c r="M23" s="25">
+        <v>813191</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="27"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="25"/>
+    </row>
+    <row r="25" spans="2:14" s="46" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="39"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="40">
-        <f>SUM(H4:H23)+D4</f>
+      <c r="C25" s="39"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="40">
+        <f>SUM(H4:H24)+D4</f>
         <v>19154932</v>
       </c>
-      <c r="I24" s="44">
-        <f>SUM(I4:I23)+(E4-D4)</f>
+      <c r="I25" s="44">
+        <f>SUM(I4:I24)+(E4-D4)</f>
         <v>2801619</v>
       </c>
-      <c r="J24" s="41">
-        <f>SUM(J4:J23)+E4</f>
+      <c r="J25" s="41">
+        <f>SUM(J4:J24)+E4</f>
         <v>21956551</v>
       </c>
-      <c r="K24" s="38">
-        <f>SUM(K4:K23)</f>
-        <v>949.3</v>
-      </c>
-      <c r="L24" s="45">
-        <f>H24/K24</f>
-        <v>20177.954282102604</v>
+      <c r="K25" s="38">
+        <f>SUM(K4:K24)</f>
+        <v>1009.3</v>
+      </c>
+      <c r="L25" s="45">
+        <f>H25/K25</f>
+        <v>18978.432577033589</v>
       </c>
     </row>
   </sheetData>
@@ -2265,9 +3216,10 @@
     <hyperlink ref="C18" r:id="rId8" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
     <hyperlink ref="C21" r:id="rId9" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
     <hyperlink ref="C22" r:id="rId10" display="http://data.ontotext.com/resource/leaks/ontology"/>
+    <hyperlink ref="C23" r:id="rId11" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967294" r:id="rId11"/>
-  <legacyDrawing r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967294" r:id="rId12"/>
+  <legacyDrawing r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
after the second full load
</commit_message>
<xml_diff>
--- a/leaks-load.xlsx
+++ b/leaks-load.xlsx
@@ -8,232 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="First load" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Author</author>
-  </authors>
-  <commentList>
-    <comment ref="B9" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-addresses were not linked, because they were not loaded properly beforehand</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B16" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-MUST be run after countries-link next time</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B17" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-MUST be loaded before leak-ontology.ttl</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B18" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-MUST be loaded before INSERT: edges-link.ru</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B19" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-run second time only because of the ommission of addresses load initially; should be removed for the next load</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B20" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-run second time only because of the ommission of addresses load initially; should be removed for the next load</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B21" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-run second time only because of the ommission of addresses load initially; should be removed for the next load</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B22" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-patch the ontology to provide superClassOff owl:Class for classes that are not linked to the class hierarchy; for the sake getting correct Class Hierarchy diagram. This will be reverted, when the diagram is fixed, because as is it introduces useless inference</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>file</t>
   </si>
@@ -241,21 +22,12 @@
     <t>context</t>
   </si>
   <si>
-    <t>before</t>
-  </si>
-  <si>
-    <t>after</t>
-  </si>
-  <si>
     <t>explicit</t>
   </si>
   <si>
     <t>total</t>
   </si>
   <si>
-    <t>diff</t>
-  </si>
-  <si>
     <t>impplicit</t>
   </si>
   <si>
@@ -268,9 +40,6 @@
     <t>countries-noleak.ttl</t>
   </si>
   <si>
-    <t>dbp-countries.ttl</t>
-  </si>
-  <si>
     <t>officers.ttl</t>
   </si>
   <si>
@@ -365,9 +134,6 @@
   </si>
   <si>
     <t>leaks:raw-data-addresses</t>
-  </si>
-  <si>
-    <t>….</t>
   </si>
   <si>
     <t>INSERT: see-also.ru</t>
@@ -398,7 +164,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -439,23 +205,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -464,18 +215,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -784,19 +529,6 @@
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1025,13 +757,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1039,7 +771,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1050,33 +782,35 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1092,10 +826,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1429,30 +1159,30 @@
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="52"/>
-      <c r="F2" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="54"/>
-      <c r="H2" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" s="55"/>
-      <c r="J2" s="52"/>
+      <c r="D2" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="54"/>
+      <c r="F2" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="56"/>
+      <c r="H2" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="57"/>
+      <c r="J2" s="54"/>
       <c r="K2" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="47" t="s">
-        <v>31</v>
+        <v>19</v>
+      </c>
+      <c r="M2" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="46" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1463,40 +1193,40 @@
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>7</v>
-      </c>
       <c r="J3" s="7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K3" s="11"/>
       <c r="L3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="47" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B4" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="57" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>41</v>
       </c>
       <c r="D4" s="14">
         <v>0</v>
@@ -1532,10 +1262,10 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" s="12" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D5" s="21">
         <f>F4</f>
@@ -1570,14 +1300,14 @@
         <f>H5/K5</f>
         <v>8740</v>
       </c>
-      <c r="M5" s="25"/>
+      <c r="M5" s="24"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D6" s="21">
         <f t="shared" ref="D6:D18" si="0">F5</f>
@@ -1615,10 +1345,10 @@
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D7" s="21">
         <f t="shared" si="0"/>
@@ -1656,10 +1386,10 @@
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D8" s="21">
         <f t="shared" si="0"/>
@@ -1697,10 +1427,10 @@
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D9" s="21">
         <f t="shared" si="0"/>
@@ -1738,10 +1468,10 @@
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" s="12" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D10" s="21">
         <f t="shared" si="0"/>
@@ -1776,14 +1506,14 @@
         <f t="shared" si="5"/>
         <v>37419.379844961237</v>
       </c>
-      <c r="M10" s="25"/>
+      <c r="M10" s="24"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="57" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="50" t="s">
-        <v>46</v>
+      <c r="B11" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>41</v>
       </c>
       <c r="D11" s="21">
         <f t="shared" si="0"/>
@@ -1818,19 +1548,19 @@
         <f t="shared" si="5"/>
         <v>25897.802547770701</v>
       </c>
-      <c r="M11" s="25">
+      <c r="M11" s="24">
         <v>813191</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" s="12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D12" s="21">
         <f t="shared" si="0"/>
@@ -1865,16 +1595,16 @@
         <f t="shared" si="5"/>
         <v>36575.854037267076</v>
       </c>
-      <c r="M12" s="25">
+      <c r="M12" s="24">
         <v>2355485</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="22"/>
@@ -1900,10 +1630,10 @@
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B14" s="12" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D14" s="21">
         <f t="shared" si="0"/>
@@ -1935,10 +1665,10 @@
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" s="12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D15" s="21">
         <f>F12</f>
@@ -1976,10 +1706,10 @@
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B16" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="50" t="s">
-        <v>38</v>
+        <v>26</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>34</v>
       </c>
       <c r="D16" s="21">
         <f t="shared" si="0"/>
@@ -2014,19 +1744,19 @@
         <f t="shared" si="5"/>
         <v>4427.3769542559357</v>
       </c>
-      <c r="M16" s="25">
+      <c r="M16" s="24">
         <v>764608</v>
       </c>
       <c r="N16" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B17" s="50" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="57" t="s">
-        <v>36</v>
-      </c>
       <c r="C17" s="13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D17" s="21">
         <f t="shared" si="0"/>
@@ -2061,19 +1791,19 @@
         <f t="shared" si="5"/>
         <v>46253.623188405792</v>
       </c>
-      <c r="M17" s="25">
+      <c r="M17" s="24">
         <v>319150</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>29</v>
       </c>
       <c r="D18" s="21">
         <f t="shared" si="0"/>
@@ -2108,16 +1838,16 @@
         <f t="shared" si="5"/>
         <v>14015.599534342258</v>
       </c>
-      <c r="M18" s="25">
+      <c r="M18" s="24">
         <v>1203940</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="26" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>45</v>
       </c>
       <c r="D19" s="21">
         <f t="shared" ref="D19" si="6">F18</f>
@@ -2152,16 +1882,16 @@
         <f t="shared" ref="L19" si="10">H19/K19</f>
         <v>16902.5</v>
       </c>
-      <c r="M19" s="25">
+      <c r="M19" s="24">
         <v>1203940</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" s="12" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D20" s="21">
         <f>F18</f>
@@ -2198,63 +1928,63 @@
       </c>
     </row>
     <row r="21" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="27"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="25"/>
-    </row>
-    <row r="22" spans="2:14" s="46" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="40">
+      <c r="B21" s="26"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="24"/>
+    </row>
+    <row r="22" spans="2:14" s="45" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="38"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="39">
         <f>SUM(H4:H21)+D4</f>
         <v>19420897</v>
       </c>
-      <c r="I22" s="44">
+      <c r="I22" s="43">
         <f>SUM(I4:I21)+(E4-D4)</f>
         <v>3140417</v>
       </c>
-      <c r="J22" s="41">
+      <c r="J22" s="40">
         <f>SUM(J4:J21)+E4</f>
         <v>22561314</v>
       </c>
-      <c r="K22" s="38">
+      <c r="K22" s="37">
         <f>SUM(K4:K21)</f>
         <v>732.80000000000007</v>
       </c>
-      <c r="L22" s="45">
+      <c r="L22" s="44">
         <f>H22/K22</f>
         <v>26502.315775109168</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B25" s="56"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B26" s="56"/>
-      <c r="C26" s="58"/>
-      <c r="D26" s="59"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="52"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B27" s="56"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2276,950 +2006,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967294" r:id="rId10"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="1.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="51" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="52"/>
-      <c r="F2" s="53" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="54"/>
-      <c r="H2" s="51" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="55"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="47" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" s="48" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="14">
-        <v>0</v>
-      </c>
-      <c r="E4" s="15">
-        <v>80</v>
-      </c>
-      <c r="F4" s="16">
-        <v>870</v>
-      </c>
-      <c r="G4" s="17">
-        <v>1272</v>
-      </c>
-      <c r="H4" s="14">
-        <f>F4-D4</f>
-        <v>870</v>
-      </c>
-      <c r="I4" s="18">
-        <f>J4-H4</f>
-        <v>322</v>
-      </c>
-      <c r="J4" s="15">
-        <f>G4-E4</f>
-        <v>1192</v>
-      </c>
-      <c r="K4" s="19">
-        <v>0.7</v>
-      </c>
-      <c r="L4" s="20">
-        <f>H4/K4</f>
-        <v>1242.8571428571429</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="21">
-        <f t="shared" ref="D5:E9" si="0">F4</f>
-        <v>870</v>
-      </c>
-      <c r="E5" s="22">
-        <f t="shared" si="0"/>
-        <v>1272</v>
-      </c>
-      <c r="F5" s="23">
-        <v>2471140</v>
-      </c>
-      <c r="G5" s="24">
-        <v>2817150</v>
-      </c>
-      <c r="H5" s="14">
-        <f>F5-D5</f>
-        <v>2470270</v>
-      </c>
-      <c r="I5" s="18">
-        <f>J5-H5</f>
-        <v>345608</v>
-      </c>
-      <c r="J5" s="15">
-        <f>G5-E5</f>
-        <v>2815878</v>
-      </c>
-      <c r="K5" s="19">
-        <v>54.6</v>
-      </c>
-      <c r="L5" s="20">
-        <f t="shared" ref="L5:L15" si="1">H5/K5</f>
-        <v>45243.040293040292</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="21">
-        <f t="shared" si="0"/>
-        <v>2471140</v>
-      </c>
-      <c r="E6" s="22">
-        <f t="shared" si="0"/>
-        <v>2817150</v>
-      </c>
-      <c r="F6" s="23">
-        <v>2668941</v>
-      </c>
-      <c r="G6" s="24">
-        <v>3038593</v>
-      </c>
-      <c r="H6" s="14">
-        <f>F6-D6</f>
-        <v>197801</v>
-      </c>
-      <c r="I6" s="18">
-        <f>J6-H6</f>
-        <v>23642</v>
-      </c>
-      <c r="J6" s="15">
-        <f>G6-E6</f>
-        <v>221443</v>
-      </c>
-      <c r="K6" s="19">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="L6" s="20">
-        <f t="shared" si="1"/>
-        <v>43000.217391304352</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="21">
-        <f t="shared" si="0"/>
-        <v>2668941</v>
-      </c>
-      <c r="E7" s="22">
-        <f t="shared" si="0"/>
-        <v>3038593</v>
-      </c>
-      <c r="F7" s="14">
-        <v>7902266</v>
-      </c>
-      <c r="G7" s="24">
-        <v>8591092</v>
-      </c>
-      <c r="H7" s="14">
-        <f>F7-D7</f>
-        <v>5233325</v>
-      </c>
-      <c r="I7" s="18">
-        <f>J7-H7</f>
-        <v>319174</v>
-      </c>
-      <c r="J7" s="15">
-        <f>G7-E7</f>
-        <v>5552499</v>
-      </c>
-      <c r="K7" s="19">
-        <v>126.3</v>
-      </c>
-      <c r="L7" s="20">
-        <f t="shared" si="1"/>
-        <v>41435.669041963578</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="21">
-        <f t="shared" si="0"/>
-        <v>7902266</v>
-      </c>
-      <c r="E8" s="22">
-        <f t="shared" si="0"/>
-        <v>8591092</v>
-      </c>
-      <c r="F8" s="23">
-        <v>12981450</v>
-      </c>
-      <c r="G8" s="24">
-        <v>13670282</v>
-      </c>
-      <c r="H8" s="14">
-        <f>F8-D8</f>
-        <v>5079184</v>
-      </c>
-      <c r="I8" s="18">
-        <f>J8-H8</f>
-        <v>6</v>
-      </c>
-      <c r="J8" s="15">
-        <f>G8-E8</f>
-        <v>5079190</v>
-      </c>
-      <c r="K8" s="19">
-        <v>123.6</v>
-      </c>
-      <c r="L8" s="20">
-        <f t="shared" si="1"/>
-        <v>41093.7216828479</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="21">
-        <f t="shared" si="0"/>
-        <v>12981450</v>
-      </c>
-      <c r="E9" s="22">
-        <f t="shared" si="0"/>
-        <v>13670282</v>
-      </c>
-      <c r="F9" s="23">
-        <v>14937999</v>
-      </c>
-      <c r="G9" s="24">
-        <v>15626835</v>
-      </c>
-      <c r="H9" s="14">
-        <f t="shared" ref="H9:H15" si="2">F9-D9</f>
-        <v>1956549</v>
-      </c>
-      <c r="I9" s="18">
-        <f t="shared" ref="I9:I15" si="3">J9-H9</f>
-        <v>4</v>
-      </c>
-      <c r="J9" s="15">
-        <f t="shared" ref="J9:J15" si="4">G9-E9</f>
-        <v>1956553</v>
-      </c>
-      <c r="K9" s="19">
-        <v>49.5</v>
-      </c>
-      <c r="L9" s="20">
-        <f t="shared" si="1"/>
-        <v>39526.242424242424</v>
-      </c>
-      <c r="M9" s="25">
-        <v>1956549</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="20"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="20"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="21">
-        <f>F9</f>
-        <v>14937999</v>
-      </c>
-      <c r="E12" s="22">
-        <f>G9</f>
-        <v>15626835</v>
-      </c>
-      <c r="F12" s="23">
-        <v>14939032</v>
-      </c>
-      <c r="G12" s="24">
-        <v>15628207</v>
-      </c>
-      <c r="H12" s="14">
-        <f t="shared" si="2"/>
-        <v>1033</v>
-      </c>
-      <c r="I12" s="18">
-        <f t="shared" si="3"/>
-        <v>339</v>
-      </c>
-      <c r="J12" s="15">
-        <f t="shared" si="4"/>
-        <v>1372</v>
-      </c>
-      <c r="K12" s="19">
-        <v>0.2</v>
-      </c>
-      <c r="L12" s="20">
-        <f t="shared" si="1"/>
-        <v>5165</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="21">
-        <f>F12</f>
-        <v>14939032</v>
-      </c>
-      <c r="E13" s="22">
-        <f>G12</f>
-        <v>15628207</v>
-      </c>
-      <c r="F13" s="23">
-        <v>15579732</v>
-      </c>
-      <c r="G13" s="24">
-        <v>16590188</v>
-      </c>
-      <c r="H13" s="14">
-        <f>F13-D13</f>
-        <v>640700</v>
-      </c>
-      <c r="I13" s="18">
-        <f>J13-H13</f>
-        <v>321281</v>
-      </c>
-      <c r="J13" s="15">
-        <f>G13-E13</f>
-        <v>961981</v>
-      </c>
-      <c r="K13" s="19">
-        <v>136.4</v>
-      </c>
-      <c r="L13" s="20">
-        <f>H13/K13</f>
-        <v>4697.2140762463341</v>
-      </c>
-      <c r="M13" s="25">
-        <f>640700</f>
-        <v>640700</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="21">
-        <f t="shared" ref="D14:E20" si="5">F13</f>
-        <v>15579732</v>
-      </c>
-      <c r="E14" s="22">
-        <f t="shared" si="5"/>
-        <v>16590188</v>
-      </c>
-      <c r="F14" s="23">
-        <v>16142326</v>
-      </c>
-      <c r="G14" s="24">
-        <v>17235242</v>
-      </c>
-      <c r="H14" s="14">
-        <f t="shared" si="2"/>
-        <v>562594</v>
-      </c>
-      <c r="I14" s="18">
-        <f t="shared" si="3"/>
-        <v>82460</v>
-      </c>
-      <c r="J14" s="15">
-        <f t="shared" si="4"/>
-        <v>645054</v>
-      </c>
-      <c r="K14" s="19">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="L14" s="20">
-        <f t="shared" si="1"/>
-        <v>29766.878306878309</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="21">
-        <f t="shared" si="5"/>
-        <v>16142326</v>
-      </c>
-      <c r="E15" s="22">
-        <f t="shared" si="5"/>
-        <v>17235242</v>
-      </c>
-      <c r="F15" s="23">
-        <v>17147475</v>
-      </c>
-      <c r="G15" s="24">
-        <v>19758781</v>
-      </c>
-      <c r="H15" s="14">
-        <f t="shared" si="2"/>
-        <v>1005149</v>
-      </c>
-      <c r="I15" s="18">
-        <f t="shared" si="3"/>
-        <v>1518390</v>
-      </c>
-      <c r="J15" s="15">
-        <f t="shared" si="4"/>
-        <v>2523539</v>
-      </c>
-      <c r="K15" s="19">
-        <v>67.099999999999994</v>
-      </c>
-      <c r="L15" s="20">
-        <f t="shared" si="1"/>
-        <v>14979.865871833086</v>
-      </c>
-      <c r="M15" s="25">
-        <f>1004149</f>
-        <v>1004149</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="21">
-        <f t="shared" si="5"/>
-        <v>17147475</v>
-      </c>
-      <c r="E16" s="22">
-        <f t="shared" si="5"/>
-        <v>19758781</v>
-      </c>
-      <c r="F16" s="23">
-        <v>17466625</v>
-      </c>
-      <c r="G16" s="23">
-        <v>20077933</v>
-      </c>
-      <c r="H16" s="14">
-        <f>F16-D16</f>
-        <v>319150</v>
-      </c>
-      <c r="I16" s="18">
-        <f>J16-H16</f>
-        <v>2</v>
-      </c>
-      <c r="J16" s="15">
-        <f>G16-E16</f>
-        <v>319152</v>
-      </c>
-      <c r="K16" s="19">
-        <v>136.4</v>
-      </c>
-      <c r="L16" s="20">
-        <f>H16/K16</f>
-        <v>2339.8093841642226</v>
-      </c>
-      <c r="M16" s="25">
-        <f>319150</f>
-        <v>319150</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="49" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="21">
-        <f t="shared" si="5"/>
-        <v>17466625</v>
-      </c>
-      <c r="E17" s="22">
-        <f t="shared" si="5"/>
-        <v>20077933</v>
-      </c>
-      <c r="F17" s="23">
-        <v>17466877</v>
-      </c>
-      <c r="G17" s="23">
-        <v>20078985</v>
-      </c>
-      <c r="H17" s="14">
-        <f>F17-D17</f>
-        <v>252</v>
-      </c>
-      <c r="I17" s="18">
-        <f>J17-H17</f>
-        <v>800</v>
-      </c>
-      <c r="J17" s="15">
-        <f>G17-E17</f>
-        <v>1052</v>
-      </c>
-      <c r="K17" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="L17" s="20">
-        <f>H17/K17</f>
-        <v>2520</v>
-      </c>
-      <c r="M17" s="25"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="49" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="21">
-        <f t="shared" si="5"/>
-        <v>17466877</v>
-      </c>
-      <c r="E18" s="22">
-        <f t="shared" si="5"/>
-        <v>20078985</v>
-      </c>
-      <c r="F18" s="23">
-        <v>18432297</v>
-      </c>
-      <c r="G18" s="23">
-        <v>21169222</v>
-      </c>
-      <c r="H18" s="14">
-        <f>F18-D18</f>
-        <v>965420</v>
-      </c>
-      <c r="I18" s="18">
-        <f>J18-H18</f>
-        <v>124817</v>
-      </c>
-      <c r="J18" s="15">
-        <f>G18-E18</f>
-        <v>1090237</v>
-      </c>
-      <c r="K18" s="19">
-        <v>31.3</v>
-      </c>
-      <c r="L18" s="20">
-        <f>H18/K18</f>
-        <v>30844.089456869009</v>
-      </c>
-      <c r="M18" s="25"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="49" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="21">
-        <f t="shared" si="5"/>
-        <v>18432297</v>
-      </c>
-      <c r="E19" s="22">
-        <f t="shared" si="5"/>
-        <v>21169222</v>
-      </c>
-      <c r="F19" s="23">
-        <v>18831233</v>
-      </c>
-      <c r="G19" s="24">
-        <v>21568158</v>
-      </c>
-      <c r="H19" s="14">
-        <f t="shared" ref="H19:H20" si="6">F19-D19</f>
-        <v>398936</v>
-      </c>
-      <c r="I19" s="18">
-        <f t="shared" ref="I19:I20" si="7">J19-H19</f>
-        <v>0</v>
-      </c>
-      <c r="J19" s="15">
-        <f t="shared" ref="J19:J20" si="8">G19-E19</f>
-        <v>398936</v>
-      </c>
-      <c r="K19" s="19">
-        <v>28.5</v>
-      </c>
-      <c r="L19" s="20">
-        <f t="shared" ref="L19:L20" si="9">H19/K19</f>
-        <v>13997.754385964912</v>
-      </c>
-      <c r="M19" s="25">
-        <v>398936</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="21">
-        <f t="shared" si="5"/>
-        <v>18831233</v>
-      </c>
-      <c r="E20" s="22">
-        <f t="shared" si="5"/>
-        <v>21568158</v>
-      </c>
-      <c r="F20" s="23">
-        <v>19031024</v>
-      </c>
-      <c r="G20" s="24">
-        <v>21769051</v>
-      </c>
-      <c r="H20" s="14">
-        <f t="shared" si="6"/>
-        <v>199791</v>
-      </c>
-      <c r="I20" s="18">
-        <f t="shared" si="7"/>
-        <v>1102</v>
-      </c>
-      <c r="J20" s="15">
-        <f t="shared" si="8"/>
-        <v>200893</v>
-      </c>
-      <c r="K20" s="19">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="L20" s="20">
-        <f t="shared" si="9"/>
-        <v>11038.17679558011</v>
-      </c>
-      <c r="M20" s="25">
-        <v>199791</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B21" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="21">
-        <f>F20</f>
-        <v>19031024</v>
-      </c>
-      <c r="E21" s="22">
-        <f>G20</f>
-        <v>21769051</v>
-      </c>
-      <c r="F21" s="23">
-        <v>19154932</v>
-      </c>
-      <c r="G21" s="24">
-        <v>21956551</v>
-      </c>
-      <c r="H21" s="14">
-        <f>F21-D21</f>
-        <v>123908</v>
-      </c>
-      <c r="I21" s="18">
-        <f>J21-H21</f>
-        <v>63592</v>
-      </c>
-      <c r="J21" s="15">
-        <f>G21-E21</f>
-        <v>187500</v>
-      </c>
-      <c r="K21" s="19">
-        <v>153</v>
-      </c>
-      <c r="L21" s="20">
-        <f>H21/K21</f>
-        <v>809.85620915032678</v>
-      </c>
-      <c r="M21" s="25">
-        <v>123908</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="49" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="15"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="20"/>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B23" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="50" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="21">
-        <f>F22</f>
-        <v>0</v>
-      </c>
-      <c r="E23" s="22">
-        <f>G22</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="23"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="14">
-        <f>F23-D23</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="18">
-        <f>J23-H23</f>
-        <v>0</v>
-      </c>
-      <c r="J23" s="15">
-        <f>G23-E23</f>
-        <v>0</v>
-      </c>
-      <c r="K23" s="19">
-        <v>60</v>
-      </c>
-      <c r="L23" s="20">
-        <f>H23/K23</f>
-        <v>0</v>
-      </c>
-      <c r="M23" s="25">
-        <v>813191</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="27"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="37"/>
-      <c r="M24" s="25"/>
-    </row>
-    <row r="25" spans="2:14" s="46" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="39"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="40">
-        <f>SUM(H4:H24)+D4</f>
-        <v>19154932</v>
-      </c>
-      <c r="I25" s="44">
-        <f>SUM(I4:I24)+(E4-D4)</f>
-        <v>2801619</v>
-      </c>
-      <c r="J25" s="41">
-        <f>SUM(J4:J24)+E4</f>
-        <v>21956551</v>
-      </c>
-      <c r="K25" s="38">
-        <f>SUM(K4:K24)</f>
-        <v>1009.3</v>
-      </c>
-      <c r="L25" s="45">
-        <f>H25/K25</f>
-        <v>18978.432577033589</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:J2"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" display="http://data.ontotext.com/resource/leaks/raw-data"/>
-    <hyperlink ref="C10" r:id="rId2" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
-    <hyperlink ref="C4" r:id="rId3" display="http://data.ontotext.com/resource/leaks/ontology"/>
-    <hyperlink ref="C6:C8" r:id="rId4" display="http://data.ontotext.com/resource/leaks/raw-data"/>
-    <hyperlink ref="C11:C14" r:id="rId5" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
-    <hyperlink ref="C16" r:id="rId6" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
-    <hyperlink ref="C17" r:id="rId7" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
-    <hyperlink ref="C18" r:id="rId8" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
-    <hyperlink ref="C21" r:id="rId9" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
-    <hyperlink ref="C22" r:id="rId10" display="http://data.ontotext.com/resource/leaks/ontology"/>
-    <hyperlink ref="C23" r:id="rId11" display="http://data.ontotext.com/resource/leaks/country-mapping"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967294" r:id="rId12"/>
-  <legacyDrawing r:id="rId13"/>
-</worksheet>
 </file>
</xml_diff>